<commit_message>
Added silkscreen, BOM parts
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Full Instrument" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
   <si>
     <t>Number</t>
   </si>
@@ -175,7 +175,52 @@
     <t>Arduino Pro Mini</t>
   </si>
   <si>
-    <t>Headers</t>
+    <t>Shipping Costs Not Included!</t>
+  </si>
+  <si>
+    <t>DEV-11114</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/11114</t>
+  </si>
+  <si>
+    <t>3.3V/8MHz Version</t>
+  </si>
+  <si>
+    <t>Ebay</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/High-Quality-Humidity-Sensor-SHT21-Breakout-Board-GY-21-/281654379137</t>
+  </si>
+  <si>
+    <t>May need alternates. Not reliable source</t>
+  </si>
+  <si>
+    <t>Break Away Headers - Straight</t>
+  </si>
+  <si>
+    <t>PRT-00116</t>
+  </si>
+  <si>
+    <t>40-Pin 0.1" Through Hole Header</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/116</t>
+  </si>
+  <si>
+    <t>Comes in strips of 40, currently only need 34. Prices will be updated once precise count is established</t>
+  </si>
+  <si>
+    <t>Sensor Headers - Add to full instrument</t>
+  </si>
+  <si>
+    <t>Jumper Wires - Add to full instrument</t>
+  </si>
+  <si>
+    <t>Shield Resistors</t>
+  </si>
+  <si>
+    <t>Shield LEDs</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1101,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1074,8 +1119,8 @@
     <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="79.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.1640625" customWidth="1"/>
+    <col min="14" max="14" width="86.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1220,28 +1265,42 @@
       <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="39">
+        <v>11.2</v>
+      </c>
       <c r="F5" s="26">
         <f t="shared" ref="F5:F30" si="0">D5*E5</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="21"/>
+        <v>11.2</v>
+      </c>
+      <c r="G5" s="21">
+        <v>11.2</v>
+      </c>
       <c r="H5" s="20">
         <f t="shared" ref="H5:H30" si="1">G5*D5*10</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="21"/>
+        <v>112</v>
+      </c>
+      <c r="I5" s="21">
+        <v>11.2</v>
+      </c>
       <c r="J5" s="20">
         <f t="shared" ref="J5:J30" si="2">I5*D5*25</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
+        <v>280</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="M5" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="19"/>
-      <c r="O5" s="45"/>
+      <c r="N5" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="45" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
@@ -1919,21 +1978,21 @@
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
-        <v>16.45</v>
+        <v>27.65</v>
       </c>
       <c r="G31" s="24" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="24">
         <f>SUM(H4:H30)</f>
-        <v>164.5</v>
+        <v>276.5</v>
       </c>
       <c r="I31" s="24" t="s">
         <v>16</v>
       </c>
       <c r="J31" s="24">
         <f>SUM(J4:J30)</f>
-        <v>411.25</v>
+        <v>691.25</v>
       </c>
       <c r="M31" s="30"/>
     </row>
@@ -1943,21 +2002,21 @@
       </c>
       <c r="F32" s="24">
         <f>F31</f>
-        <v>16.45</v>
+        <v>27.65</v>
       </c>
       <c r="G32" t="s">
         <v>17</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
-        <v>16.45</v>
+        <v>27.65</v>
       </c>
       <c r="I32" t="s">
         <v>17</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
-        <v>16.45</v>
+        <v>27.65</v>
       </c>
       <c r="M32" s="30"/>
     </row>
@@ -1979,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1997,9 +2056,9 @@
     <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.83203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28" style="30" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="130.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="83.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2010,7 +2069,9 @@
       <c r="C1" s="1">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
@@ -2089,28 +2150,48 @@
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="37"/>
+      <c r="C4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="37">
+        <v>9.9499999999999993</v>
+      </c>
       <c r="F4" s="38">
         <f t="shared" ref="F4" si="0">D4*E4</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="42"/>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="G4" s="42">
+        <v>9.4499999999999993</v>
+      </c>
       <c r="H4" s="43">
         <f t="shared" ref="H4" si="1">D4*G4*10</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="42"/>
+        <v>94.5</v>
+      </c>
+      <c r="I4" s="42">
+        <v>8.9600000000000009</v>
+      </c>
       <c r="J4" s="43">
         <f t="shared" ref="J4" si="2">D4*I4*25</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="44"/>
+        <v>224.00000000000003</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="44" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
@@ -2291,28 +2372,48 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="39"/>
+      <c r="C9" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="39">
+        <v>1.5</v>
+      </c>
       <c r="F9" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="21"/>
+        <v>1.5</v>
+      </c>
+      <c r="G9" s="21">
+        <v>1.5</v>
+      </c>
       <c r="H9" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="21"/>
+        <v>15</v>
+      </c>
+      <c r="I9" s="21">
+        <v>1.43</v>
+      </c>
       <c r="J9" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="45"/>
+        <v>35.75</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="M9" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="O9" s="45" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
@@ -2866,21 +2967,21 @@
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
-        <v>4.49</v>
+        <v>15.94</v>
       </c>
       <c r="G31" s="24" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="24">
         <f>SUM(H4:H30)</f>
-        <v>44.9</v>
+        <v>154.4</v>
       </c>
       <c r="I31" s="24" t="s">
         <v>16</v>
       </c>
       <c r="J31" s="24">
         <f>SUM(J4:J30)</f>
-        <v>102.75</v>
+        <v>362.5</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -2889,21 +2990,21 @@
       </c>
       <c r="F32" s="24">
         <f>F31</f>
-        <v>4.49</v>
+        <v>15.94</v>
       </c>
       <c r="G32" t="s">
         <v>17</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
-        <v>4.49</v>
+        <v>15.440000000000001</v>
       </c>
       <c r="I32" t="s">
         <v>17</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
-        <v>4.1100000000000003</v>
+        <v>14.5</v>
       </c>
     </row>
   </sheetData>
@@ -2927,10 +3028,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2940,14 +3041,24 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-    </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many changes and added gerber files
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Full Instrument" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="83">
   <si>
     <t>Number</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Part Name</t>
   </si>
   <si>
-    <t>Cost/Unit</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -217,10 +214,67 @@
     <t>Jumper Wires - Add to full instrument</t>
   </si>
   <si>
-    <t>Shield Resistors</t>
-  </si>
-  <si>
-    <t>Shield LEDs</t>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>604-WP710A10ID</t>
+  </si>
+  <si>
+    <t>T-1 (3 mm)</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Kingbright/WP710A10ID/?qs=sGAEpiMZZMtmwHDZQCdlqbkQSv8HD28QuawgpDquR1I%3d</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>604-WP710A10GD</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Kingbright/WP710A10GD/?qs=sGAEpiMZZMtmwHDZQCdlqbkQSv8HD28Qk0jBElTDvNI%3d</t>
+  </si>
+  <si>
+    <t>270 Ohm Resistor</t>
+  </si>
+  <si>
+    <t>2V forward voltage</t>
+  </si>
+  <si>
+    <t>2.2V forward voltage</t>
+  </si>
+  <si>
+    <t>220 Ohm Resistor</t>
+  </si>
+  <si>
+    <t>3.3V supply, 2.2V voltage drop, 5mA forward current. For green LED</t>
+  </si>
+  <si>
+    <t>594-5063JD270R0F</t>
+  </si>
+  <si>
+    <t>Cost/Part</t>
+  </si>
+  <si>
+    <t>0207</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Beyschlag/MBA02040C2700FC100/?qs=sGAEpiMZZMsPqMdJzcrNwh8o%2ffOfPMK399V4azr1c3I%3d</t>
+  </si>
+  <si>
+    <t>3.3V supply, 2V voltage drop, 5mA forward current. For red LED. Check package size</t>
+  </si>
+  <si>
+    <t>594-5063JD220R0F</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-BC-Components/MBA02040C2200FC100/?qs=sGAEpiMZZMsPqMdJzcrNwjHuaZ59ATdsAyWvarnMzXw%3d</t>
+  </si>
+  <si>
+    <t>Battery voltage divider resistors</t>
   </si>
 </sst>
 </file>
@@ -273,7 +327,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -575,17 +629,6 @@
       <top style="double">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -662,7 +705,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -705,21 +748,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1101,7 +1143,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1124,10 +1166,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="50"/>
+      <c r="A1" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="49"/>
       <c r="C1" s="1">
         <v>1</v>
       </c>
@@ -1135,32 +1177,32 @@
       <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="53"/>
+      <c r="G2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="55" t="s">
+      <c r="H2" s="53"/>
+      <c r="I2" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="51" t="s">
+      <c r="J2" s="53"/>
+      <c r="K2" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="47" t="s">
-        <v>28</v>
+      <c r="L2" s="51"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="46" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1168,104 +1210,104 @@
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="14" t="s">
+      <c r="N3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" s="48"/>
+      <c r="O3" s="47"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="36">
         <v>6.5</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="37">
         <f>D4*E4</f>
         <v>6.5</v>
       </c>
-      <c r="G4" s="42">
+      <c r="G4" s="41">
         <v>6.5</v>
       </c>
-      <c r="H4" s="43">
+      <c r="H4" s="42">
         <f>G4*D4*10</f>
         <v>65</v>
       </c>
-      <c r="I4" s="42">
+      <c r="I4" s="41">
         <v>6.5</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="42">
         <f>I4*D4*25</f>
         <v>162.5</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="29" t="s">
+      <c r="N4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="44"/>
+      <c r="O4" s="43"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="38">
         <v>11.2</v>
       </c>
       <c r="F5" s="26">
@@ -1287,33 +1329,33 @@
         <v>280</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="19" t="s">
+      <c r="O5" s="44" t="s">
         <v>54</v>
-      </c>
-      <c r="O5" s="45" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="38">
         <v>9.9499999999999993</v>
       </c>
       <c r="F6" s="26">
@@ -1335,25 +1377,25 @@
         <v>248.74999999999997</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="O6" s="45"/>
+      <c r="O6" s="44"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="25"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="39"/>
+      <c r="E7" s="38"/>
       <c r="F7" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1372,14 +1414,14 @@
       <c r="L7" s="3"/>
       <c r="M7" s="32"/>
       <c r="N7" s="19"/>
-      <c r="O7" s="45"/>
+      <c r="O7" s="44"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="39"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1398,14 +1440,14 @@
       <c r="L8" s="3"/>
       <c r="M8" s="32"/>
       <c r="N8" s="19"/>
-      <c r="O8" s="45"/>
+      <c r="O8" s="44"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="25"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="39"/>
+      <c r="E9" s="38"/>
       <c r="F9" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1424,14 +1466,14 @@
       <c r="L9" s="3"/>
       <c r="M9" s="32"/>
       <c r="N9" s="19"/>
-      <c r="O9" s="45"/>
+      <c r="O9" s="44"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="25"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="39"/>
+      <c r="E10" s="38"/>
       <c r="F10" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1450,14 +1492,14 @@
       <c r="L10" s="3"/>
       <c r="M10" s="32"/>
       <c r="N10" s="19"/>
-      <c r="O10" s="45"/>
+      <c r="O10" s="44"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="39"/>
+      <c r="E11" s="38"/>
       <c r="F11" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1476,14 +1518,14 @@
       <c r="L11" s="3"/>
       <c r="M11" s="32"/>
       <c r="N11" s="19"/>
-      <c r="O11" s="45"/>
+      <c r="O11" s="44"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="34"/>
       <c r="C12" s="25"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="39"/>
+      <c r="E12" s="38"/>
       <c r="F12" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1502,14 +1544,14 @@
       <c r="L12" s="3"/>
       <c r="M12" s="29"/>
       <c r="N12" s="19"/>
-      <c r="O12" s="45"/>
+      <c r="O12" s="44"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="39"/>
+      <c r="E13" s="38"/>
       <c r="F13" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1528,14 +1570,14 @@
       <c r="L13" s="3"/>
       <c r="M13" s="29"/>
       <c r="N13" s="19"/>
-      <c r="O13" s="45"/>
+      <c r="O13" s="44"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="39"/>
+      <c r="E14" s="38"/>
       <c r="F14" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1554,14 +1596,14 @@
       <c r="L14" s="3"/>
       <c r="M14" s="29"/>
       <c r="N14" s="19"/>
-      <c r="O14" s="45"/>
+      <c r="O14" s="44"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="39"/>
+      <c r="E15" s="38"/>
       <c r="F15" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1580,14 +1622,14 @@
       <c r="L15" s="3"/>
       <c r="M15" s="29"/>
       <c r="N15" s="19"/>
-      <c r="O15" s="45"/>
+      <c r="O15" s="44"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="39"/>
+      <c r="E16" s="38"/>
       <c r="F16" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1606,14 +1648,14 @@
       <c r="L16" s="3"/>
       <c r="M16" s="32"/>
       <c r="N16" s="27"/>
-      <c r="O16" s="45"/>
+      <c r="O16" s="44"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="39"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1632,14 +1674,14 @@
       <c r="L17" s="3"/>
       <c r="M17" s="29"/>
       <c r="N17" s="19"/>
-      <c r="O17" s="45"/>
+      <c r="O17" s="44"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="39"/>
+      <c r="E18" s="38"/>
       <c r="F18" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1658,14 +1700,14 @@
       <c r="L18" s="3"/>
       <c r="M18" s="29"/>
       <c r="N18" s="19"/>
-      <c r="O18" s="45"/>
+      <c r="O18" s="44"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="34"/>
       <c r="C19" s="25"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="39"/>
+      <c r="E19" s="38"/>
       <c r="F19" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1684,14 +1726,14 @@
       <c r="L19" s="3"/>
       <c r="M19" s="29"/>
       <c r="N19" s="19"/>
-      <c r="O19" s="45"/>
+      <c r="O19" s="44"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="39"/>
+      <c r="E20" s="38"/>
       <c r="F20" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1710,14 +1752,14 @@
       <c r="L20" s="3"/>
       <c r="M20" s="29"/>
       <c r="N20" s="19"/>
-      <c r="O20" s="45"/>
+      <c r="O20" s="44"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="39"/>
+      <c r="E21" s="38"/>
       <c r="F21" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1736,14 +1778,14 @@
       <c r="L21" s="3"/>
       <c r="M21" s="29"/>
       <c r="N21" s="19"/>
-      <c r="O21" s="45"/>
+      <c r="O21" s="44"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="39"/>
+      <c r="E22" s="38"/>
       <c r="F22" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1762,14 +1804,14 @@
       <c r="L22" s="3"/>
       <c r="M22" s="29"/>
       <c r="N22" s="19"/>
-      <c r="O22" s="45"/>
+      <c r="O22" s="44"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="39"/>
+      <c r="E23" s="38"/>
       <c r="F23" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1788,14 +1830,14 @@
       <c r="L23" s="3"/>
       <c r="M23" s="29"/>
       <c r="N23" s="19"/>
-      <c r="O23" s="45"/>
+      <c r="O23" s="44"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="39"/>
+      <c r="E24" s="38"/>
       <c r="F24" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1814,14 +1856,14 @@
       <c r="L24" s="3"/>
       <c r="M24" s="29"/>
       <c r="N24" s="19"/>
-      <c r="O24" s="45"/>
+      <c r="O24" s="44"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="25"/>
       <c r="C25" s="25"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="39"/>
+      <c r="E25" s="38"/>
       <c r="F25" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1840,14 +1882,14 @@
       <c r="L25" s="3"/>
       <c r="M25" s="29"/>
       <c r="N25" s="19"/>
-      <c r="O25" s="45"/>
+      <c r="O25" s="44"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="39"/>
+      <c r="E26" s="38"/>
       <c r="F26" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1866,14 +1908,14 @@
       <c r="L26" s="3"/>
       <c r="M26" s="29"/>
       <c r="N26" s="4"/>
-      <c r="O26" s="45"/>
+      <c r="O26" s="44"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="39"/>
+      <c r="E27" s="38"/>
       <c r="F27" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1892,14 +1934,14 @@
       <c r="L27" s="3"/>
       <c r="M27" s="29"/>
       <c r="N27" s="4"/>
-      <c r="O27" s="45"/>
+      <c r="O27" s="44"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="39"/>
+      <c r="E28" s="38"/>
       <c r="F28" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1918,14 +1960,14 @@
       <c r="L28" s="3"/>
       <c r="M28" s="29"/>
       <c r="N28" s="4"/>
-      <c r="O28" s="45"/>
+      <c r="O28" s="44"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="39"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1944,14 +1986,14 @@
       <c r="L29" s="3"/>
       <c r="M29" s="29"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="45"/>
+      <c r="O29" s="44"/>
     </row>
     <row r="30" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
-      <c r="E30" s="40"/>
+      <c r="E30" s="39"/>
       <c r="F30" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1970,25 +2012,25 @@
       <c r="L30" s="6"/>
       <c r="M30" s="33"/>
       <c r="N30" s="7"/>
-      <c r="O30" s="46"/>
+      <c r="O30" s="45"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E31" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
         <v>27.65</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H31" s="24">
         <f>SUM(H4:H30)</f>
         <v>276.5</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J31" s="24">
         <f>SUM(J4:J30)</f>
@@ -1998,21 +2040,21 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F32" s="24">
         <f>F31</f>
         <v>27.65</v>
       </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
         <v>27.65</v>
       </c>
       <c r="I32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
@@ -2038,8 +2080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2062,44 +2104,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="50"/>
+      <c r="A1" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="49"/>
       <c r="C1" s="1">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="53"/>
+      <c r="G2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="55" t="s">
+      <c r="H2" s="53"/>
+      <c r="I2" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="51" t="s">
+      <c r="J2" s="53"/>
+      <c r="K2" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="47" t="s">
-        <v>28</v>
+      <c r="L2" s="51"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="46" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2113,96 +2155,96 @@
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="14" t="s">
+      <c r="N3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" s="48"/>
+      <c r="O3" s="47"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="36">
         <v>9.9499999999999993</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="37">
         <f t="shared" ref="F4" si="0">D4*E4</f>
         <v>9.9499999999999993</v>
       </c>
-      <c r="G4" s="42">
+      <c r="G4" s="41">
         <v>9.4499999999999993</v>
       </c>
-      <c r="H4" s="43">
+      <c r="H4" s="42">
         <f t="shared" ref="H4" si="1">D4*G4*10</f>
         <v>94.5</v>
       </c>
-      <c r="I4" s="42">
+      <c r="I4" s="41">
         <v>8.9600000000000009</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="42">
         <f t="shared" ref="J4" si="2">D4*I4*25</f>
         <v>224.00000000000003</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="19" t="s">
+      <c r="O4" s="43" t="s">
         <v>51</v>
-      </c>
-      <c r="O4" s="44" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="25"/>
       <c r="C5" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="38">
         <v>1.5</v>
       </c>
       <c r="F5" s="26">
@@ -2224,29 +2266,29 @@
         <v>35.75</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="45"/>
+      <c r="O5" s="44"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25"/>
       <c r="C6" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="38">
         <v>1.74</v>
       </c>
       <c r="F6" s="26">
@@ -2268,29 +2310,29 @@
         <v>37.25</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="45"/>
+      <c r="O6" s="44"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="38">
         <v>0.5</v>
       </c>
       <c r="F7" s="26">
@@ -2312,29 +2354,29 @@
         <v>12</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="M7" s="32" t="s">
+      <c r="N7" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="N7" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O7" s="45"/>
+      <c r="O7" s="44"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25"/>
       <c r="C8" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="38">
         <v>0.75</v>
       </c>
       <c r="F8" s="26">
@@ -2356,29 +2398,29 @@
         <v>17.75</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M8" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N8" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="O8" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="O8" s="44"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="38">
         <v>1.5</v>
       </c>
       <c r="F9" s="26">
@@ -2400,131 +2442,211 @@
         <v>35.75</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L9" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="M9" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="N9" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="N9" s="19" t="s">
+      <c r="O9" s="44" t="s">
         <v>59</v>
-      </c>
-      <c r="O9" s="45" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="39"/>
+      <c r="C10" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="38">
+        <v>0.13</v>
+      </c>
       <c r="F10" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="21"/>
+        <v>0.13</v>
+      </c>
+      <c r="G10" s="21">
+        <v>7.9000000000000001E-2</v>
+      </c>
       <c r="H10" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="21"/>
+        <v>0.79</v>
+      </c>
+      <c r="I10" s="21">
+        <v>7.9000000000000001E-2</v>
+      </c>
       <c r="J10" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="45"/>
+        <v>1.9750000000000001</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="M10" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="O10" s="44" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="39"/>
+      <c r="C11" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="38">
+        <v>0.14000000000000001</v>
+      </c>
       <c r="F11" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="21"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G11" s="21">
+        <v>8.5999999999999993E-2</v>
+      </c>
       <c r="H11" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="21"/>
+        <v>0.85999999999999988</v>
+      </c>
+      <c r="I11" s="21">
+        <v>8.5999999999999993E-2</v>
+      </c>
       <c r="J11" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="45"/>
+        <v>2.15</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="O11" s="44" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="34"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="39"/>
+      <c r="C12" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="38">
+        <v>0.13</v>
+      </c>
       <c r="F12" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="21"/>
+        <v>0.13</v>
+      </c>
+      <c r="G12" s="21">
+        <v>0.13</v>
+      </c>
       <c r="H12" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="21"/>
+        <v>1.3</v>
+      </c>
+      <c r="I12" s="21">
+        <v>0.13</v>
+      </c>
       <c r="J12" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="45"/>
+        <v>3.25</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="O12" s="44" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="39"/>
+      <c r="C13" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="38">
+        <v>0.12</v>
+      </c>
       <c r="F13" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="21"/>
+        <v>0.12</v>
+      </c>
+      <c r="G13" s="21">
+        <v>0.12</v>
+      </c>
       <c r="H13" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="21"/>
+        <v>1.2</v>
+      </c>
+      <c r="I13" s="21">
+        <v>0.12</v>
+      </c>
       <c r="J13" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="45"/>
+        <v>3</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M13" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="O13" s="44" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="39"/>
+      <c r="E14" s="38"/>
       <c r="F14" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2543,14 +2665,14 @@
       <c r="L14" s="3"/>
       <c r="M14" s="29"/>
       <c r="N14" s="19"/>
-      <c r="O14" s="45"/>
+      <c r="O14" s="44"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="39"/>
+      <c r="E15" s="38"/>
       <c r="F15" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2569,14 +2691,14 @@
       <c r="L15" s="3"/>
       <c r="M15" s="29"/>
       <c r="N15" s="19"/>
-      <c r="O15" s="45"/>
+      <c r="O15" s="44"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="39"/>
+      <c r="E16" s="38"/>
       <c r="F16" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2595,14 +2717,14 @@
       <c r="L16" s="3"/>
       <c r="M16" s="32"/>
       <c r="N16" s="27"/>
-      <c r="O16" s="45"/>
+      <c r="O16" s="44"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="39"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2621,14 +2743,14 @@
       <c r="L17" s="3"/>
       <c r="M17" s="29"/>
       <c r="N17" s="19"/>
-      <c r="O17" s="45"/>
+      <c r="O17" s="44"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="39"/>
+      <c r="E18" s="38"/>
       <c r="F18" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2647,14 +2769,14 @@
       <c r="L18" s="3"/>
       <c r="M18" s="29"/>
       <c r="N18" s="19"/>
-      <c r="O18" s="45"/>
+      <c r="O18" s="44"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="34"/>
       <c r="C19" s="25"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="39"/>
+      <c r="E19" s="38"/>
       <c r="F19" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2673,14 +2795,14 @@
       <c r="L19" s="3"/>
       <c r="M19" s="29"/>
       <c r="N19" s="19"/>
-      <c r="O19" s="45"/>
+      <c r="O19" s="44"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="39"/>
+      <c r="E20" s="38"/>
       <c r="F20" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2699,14 +2821,14 @@
       <c r="L20" s="3"/>
       <c r="M20" s="29"/>
       <c r="N20" s="19"/>
-      <c r="O20" s="45"/>
+      <c r="O20" s="44"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="39"/>
+      <c r="E21" s="38"/>
       <c r="F21" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2725,14 +2847,14 @@
       <c r="L21" s="3"/>
       <c r="M21" s="29"/>
       <c r="N21" s="19"/>
-      <c r="O21" s="45"/>
+      <c r="O21" s="44"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="39"/>
+      <c r="E22" s="38"/>
       <c r="F22" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2751,14 +2873,14 @@
       <c r="L22" s="3"/>
       <c r="M22" s="29"/>
       <c r="N22" s="19"/>
-      <c r="O22" s="45"/>
+      <c r="O22" s="44"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="39"/>
+      <c r="E23" s="38"/>
       <c r="F23" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2777,14 +2899,14 @@
       <c r="L23" s="3"/>
       <c r="M23" s="29"/>
       <c r="N23" s="19"/>
-      <c r="O23" s="45"/>
+      <c r="O23" s="44"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="39"/>
+      <c r="E24" s="38"/>
       <c r="F24" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2803,14 +2925,14 @@
       <c r="L24" s="3"/>
       <c r="M24" s="29"/>
       <c r="N24" s="19"/>
-      <c r="O24" s="45"/>
+      <c r="O24" s="44"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="25"/>
       <c r="C25" s="25"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="39"/>
+      <c r="E25" s="38"/>
       <c r="F25" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2829,14 +2951,14 @@
       <c r="L25" s="3"/>
       <c r="M25" s="29"/>
       <c r="N25" s="19"/>
-      <c r="O25" s="45"/>
+      <c r="O25" s="44"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="39"/>
+      <c r="E26" s="38"/>
       <c r="F26" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2855,14 +2977,14 @@
       <c r="L26" s="3"/>
       <c r="M26" s="29"/>
       <c r="N26" s="4"/>
-      <c r="O26" s="45"/>
+      <c r="O26" s="44"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="39"/>
+      <c r="E27" s="38"/>
       <c r="F27" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2881,14 +3003,14 @@
       <c r="L27" s="3"/>
       <c r="M27" s="29"/>
       <c r="N27" s="4"/>
-      <c r="O27" s="45"/>
+      <c r="O27" s="44"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="39"/>
+      <c r="E28" s="38"/>
       <c r="F28" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2907,14 +3029,14 @@
       <c r="L28" s="3"/>
       <c r="M28" s="29"/>
       <c r="N28" s="4"/>
-      <c r="O28" s="45"/>
+      <c r="O28" s="44"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="39"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2933,14 +3055,14 @@
       <c r="L29" s="3"/>
       <c r="M29" s="29"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="45"/>
+      <c r="O29" s="44"/>
     </row>
     <row r="30" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
-      <c r="E30" s="40"/>
+      <c r="E30" s="39"/>
       <c r="F30" s="15">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2959,52 +3081,52 @@
       <c r="L30" s="6"/>
       <c r="M30" s="33"/>
       <c r="N30" s="7"/>
-      <c r="O30" s="46"/>
+      <c r="O30" s="45"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E31" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
-        <v>15.94</v>
+        <v>16.46</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H31" s="24">
         <f>SUM(H4:H30)</f>
-        <v>154.4</v>
+        <v>158.55000000000001</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J31" s="24">
         <f>SUM(J4:J30)</f>
-        <v>362.5</v>
+        <v>372.875</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F32" s="24">
         <f>F31</f>
-        <v>15.94</v>
+        <v>16.46</v>
       </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
-        <v>15.440000000000001</v>
+        <v>15.855</v>
       </c>
       <c r="I32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
-        <v>14.5</v>
+        <v>14.914999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3023,42 +3145,40 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="M12:M13" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
-        <v>18</v>
+      <c r="A1" s="40" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.1 final, mostly finished BOM
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Full Instrument" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="116">
   <si>
     <t>Number</t>
   </si>
@@ -205,9 +205,6 @@
     <t>Sensor Headers - Add to full instrument</t>
   </si>
   <si>
-    <t>Jumper Wires - Add to full instrument</t>
-  </si>
-  <si>
     <t>Red LED</t>
   </si>
   <si>
@@ -247,30 +244,12 @@
     <t>3.3V supply, 2.2V voltage drop, 5mA forward current. For green LED</t>
   </si>
   <si>
-    <t>594-5063JD270R0F</t>
-  </si>
-  <si>
     <t>Cost/Part</t>
   </si>
   <si>
-    <t>0207</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Vishay-Beyschlag/MBA02040C2700FC100/?qs=sGAEpiMZZMsPqMdJzcrNwh8o%2ffOfPMK399V4azr1c3I%3d</t>
-  </si>
-  <si>
     <t>3.3V supply, 2V voltage drop, 5mA forward current. For red LED. Check package size</t>
   </si>
   <si>
-    <t>594-5063JD220R0F</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Vishay-BC-Components/MBA02040C2200FC100/?qs=sGAEpiMZZMsPqMdJzcrNwjHuaZ59ATdsAyWvarnMzXw%3d</t>
-  </si>
-  <si>
-    <t>Battery voltage divider resistors</t>
-  </si>
-  <si>
     <t>Real Time Clock</t>
   </si>
   <si>
@@ -296,6 +275,105 @@
   </si>
   <si>
     <t>Should also be sold at sparkfun, https://www.sparkfun.com/products/8084</t>
+  </si>
+  <si>
+    <t>AA Batteries</t>
+  </si>
+  <si>
+    <t>24k Ohm Resistor</t>
+  </si>
+  <si>
+    <t>30k Ohm Resistor</t>
+  </si>
+  <si>
+    <t>Printed Circuit Board</t>
+  </si>
+  <si>
+    <t>OshPark</t>
+  </si>
+  <si>
+    <t>Currently using OshPark Prices @ $8.45 for 2"x2.5" board ($5/in^2). Will change once quantity price is determined</t>
+  </si>
+  <si>
+    <t>Jumper Wires</t>
+  </si>
+  <si>
+    <t>Comes in packs of 20/40, currently only need 8</t>
+  </si>
+  <si>
+    <t>658-LR6XWA</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Panasonic-Battery/LR6XWA-B/?qs=sGAEpiMZZMuXcNZ31nzYhcGI0qUUgbjI14kQITT1Veg%3d</t>
+  </si>
+  <si>
+    <t>Comes in packs of 500. Digikey has same part for cheaper with smaller quantities if necessary</t>
+  </si>
+  <si>
+    <t>12BH348-GR</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Eagle-Plastic-Devices/12BH348-GR/?qs=%2fha2pyFadugRkpBjv4dscP6C0TFGxFRnCHo%252bDaSpfTs%3d</t>
+  </si>
+  <si>
+    <t>Much cheaper if bought in quantities of 100+</t>
+  </si>
+  <si>
+    <t>SD Card</t>
+  </si>
+  <si>
+    <t>Full Shield</t>
+  </si>
+  <si>
+    <t>See 'Shield Parts' Sheet for details</t>
+  </si>
+  <si>
+    <t>4x AA batteries for 6V total in series at max. Voltage divider down to 3.3V for Arduino analag read</t>
+  </si>
+  <si>
+    <t>658-CR1220</t>
+  </si>
+  <si>
+    <t>1220</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Panasonic-Battery/CR1220/?qs=sGAEpiMZZMuuBt6TL7D%2f6A7P4Pabhz5g</t>
+  </si>
+  <si>
+    <t>Much cheaper if bought in quantities of 50+</t>
+  </si>
+  <si>
+    <t>588-OK2715E-R52</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Ohmite/OK2715E-R52/?qs=sGAEpiMZZMtlubZbdhIBIJMLE6vvLglcKmeAomrNvK0%3d</t>
+  </si>
+  <si>
+    <t>588-OK2215E-R52</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Ohmite/OK2215E-R52/?qs=sGAEpiMZZMtlubZbdhIBIJMLE6vvLglcwrpJO6Dxohs%3d</t>
+  </si>
+  <si>
+    <t>603-MFR-25FTE52-24K</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Yageo/MFR-25FTE52-24K/?qs=sGAEpiMZZMsPqMdJzcrNwvki5I7GwxKeyTca%2fGdX9DM%3d</t>
+  </si>
+  <si>
+    <t>MFR-25FBF52-30K</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Yageo/MFR-25FBF52-30K/?qs=sGAEpiMZZMsPqMdJzcrNwvki5I7GwxKexr3bQCDZBCM%3d</t>
+  </si>
+  <si>
+    <t>4x AA Battery Holder</t>
+  </si>
+  <si>
+    <t>See 'Shield Parts'</t>
   </si>
 </sst>
 </file>
@@ -727,7 +805,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -808,6 +886,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1165,15 +1252,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
@@ -1184,8 +1271,8 @@
     <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="86.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="119.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="76.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1196,7 +1283,9 @@
       <c r="C1" s="1">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1242,19 +1331,19 @@
         <v>12</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F3" s="28" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>14</v>
@@ -1416,10 +1505,10 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -1446,7 +1535,7 @@
         <v>314</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="L7" s="3">
         <v>3013</v>
@@ -1455,71 +1544,111 @@
         <v>30</v>
       </c>
       <c r="N7" s="19" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="O7" s="44"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
-      <c r="E8" s="38"/>
+      <c r="E8" s="38">
+        <v>0.87</v>
+      </c>
       <c r="F8" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="21"/>
+        <v>0.87</v>
+      </c>
+      <c r="G8" s="21">
+        <v>0.78800000000000003</v>
+      </c>
       <c r="H8" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="21"/>
+        <v>7.8800000000000008</v>
+      </c>
+      <c r="I8" s="21">
+        <v>0.78800000000000003</v>
+      </c>
       <c r="J8" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="44"/>
+        <v>19.7</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="M8" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="O8" s="44" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="38"/>
+      <c r="B9" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4">
+        <v>8</v>
+      </c>
+      <c r="E9" s="38">
+        <v>0.22500000000000001</v>
+      </c>
       <c r="F9" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="21"/>
+        <v>1.8</v>
+      </c>
+      <c r="G9" s="21">
+        <v>0.22500000000000001</v>
+      </c>
       <c r="H9" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="21"/>
+        <v>18</v>
+      </c>
+      <c r="I9" s="21">
+        <v>0.22500000000000001</v>
+      </c>
       <c r="J9" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="44"/>
+        <v>45</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M9" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="O9" s="44" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
+      <c r="B10" s="25" t="s">
+        <v>89</v>
+      </c>
       <c r="C10" s="25"/>
       <c r="D10" s="4"/>
       <c r="E10" s="38"/>
@@ -1537,41 +1666,69 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K10" s="2"/>
+      <c r="K10" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="L10" s="3"/>
       <c r="M10" s="32"/>
       <c r="N10" s="19"/>
-      <c r="O10" s="44"/>
+      <c r="O10" s="44" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="38"/>
+      <c r="B11" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="38">
+        <v>1.28</v>
+      </c>
       <c r="F11" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="21"/>
+        <v>2.56</v>
+      </c>
+      <c r="G11" s="21">
+        <v>1.18</v>
+      </c>
       <c r="H11" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="21"/>
+        <v>23.599999999999998</v>
+      </c>
+      <c r="I11" s="21">
+        <v>1.18</v>
+      </c>
       <c r="J11" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="44"/>
+        <v>59</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="O11" s="44" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="34"/>
+      <c r="B12" s="34" t="s">
+        <v>98</v>
+      </c>
       <c r="C12" s="25"/>
       <c r="D12" s="4"/>
       <c r="E12" s="38"/>
@@ -1597,29 +1754,52 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="38"/>
+      <c r="B13" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="38">
+        <f>'Shield Parts'!$F$32</f>
+        <v>24.820000000000004</v>
+      </c>
       <c r="F13" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="21"/>
+        <f t="shared" ref="F13" si="3">D13*E13</f>
+        <v>24.820000000000004</v>
+      </c>
+      <c r="G13" s="21">
+        <f>'Shield Parts'!$H$32</f>
+        <v>23.958999999999996</v>
+      </c>
       <c r="H13" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="21"/>
+        <f t="shared" ref="H13" si="4">G13*D13*10</f>
+        <v>239.58999999999997</v>
+      </c>
+      <c r="I13" s="21">
+        <f>'Shield Parts'!$J$32</f>
+        <v>22.98</v>
+      </c>
       <c r="J13" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="29"/>
+        <f t="shared" ref="J13" si="5">I13*D13*25</f>
+        <v>574.5</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="29" t="s">
+        <v>18</v>
+      </c>
       <c r="N13" s="19"/>
-      <c r="O13" s="44"/>
+      <c r="O13" s="44" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -2038,30 +2218,30 @@
       <c r="O29" s="44"/>
     </row>
     <row r="30" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="15">
+      <c r="A30" s="56"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="60">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G30" s="23"/>
-      <c r="H30" s="22">
+      <c r="G30" s="61"/>
+      <c r="H30" s="62">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I30" s="23"/>
-      <c r="J30" s="22">
+      <c r="I30" s="61"/>
+      <c r="J30" s="62">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K30" s="5"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="45"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="63"/>
+      <c r="N30" s="58"/>
+      <c r="O30" s="64"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E31" s="24" t="s">
@@ -2069,21 +2249,21 @@
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
-        <v>41.599999999999994</v>
+        <v>71.649999999999991</v>
       </c>
       <c r="G31" s="24" t="s">
         <v>15</v>
       </c>
       <c r="H31" s="24">
         <f>SUM(H4:H30)</f>
-        <v>402.1</v>
+        <v>691.17000000000007</v>
       </c>
       <c r="I31" s="24" t="s">
         <v>15</v>
       </c>
       <c r="J31" s="24">
         <f>SUM(J4:J30)</f>
-        <v>1005.25</v>
+        <v>1703.45</v>
       </c>
       <c r="M31" s="30"/>
     </row>
@@ -2093,21 +2273,21 @@
       </c>
       <c r="F32" s="24">
         <f>F31</f>
-        <v>41.599999999999994</v>
+        <v>71.649999999999991</v>
       </c>
       <c r="G32" t="s">
         <v>16</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
-        <v>40.21</v>
+        <v>69.117000000000004</v>
       </c>
       <c r="I32" t="s">
         <v>16</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
-        <v>40.21</v>
+        <v>68.138000000000005</v>
       </c>
       <c r="M32" s="30"/>
     </row>
@@ -2129,8 +2309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2146,10 +2326,10 @@
     <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="28" style="30" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="130.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="83.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="94" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2207,19 +2387,19 @@
         <v>12</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F3" s="28" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>14</v>
@@ -2447,19 +2627,19 @@
         <v>8.9249999999999989</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="M8" s="32" t="s">
         <v>18</v>
       </c>
       <c r="N8" s="19" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="O8" s="44" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -2512,7 +2692,7 @@
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -2539,26 +2719,26 @@
         <v>1.9750000000000001</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="N10" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="N10" s="19" t="s">
-        <v>64</v>
-      </c>
       <c r="O10" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -2585,72 +2765,72 @@
         <v>2.15</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="M11" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>67</v>
-      </c>
       <c r="O11" s="44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="34"/>
       <c r="C12" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
       </c>
       <c r="E12" s="38">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F12" s="26">
         <f t="shared" si="4"/>
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="G12" s="21">
-        <v>0.13</v>
+        <v>0.02</v>
       </c>
       <c r="H12" s="20">
         <f t="shared" si="3"/>
-        <v>1.3</v>
+        <v>0.2</v>
       </c>
       <c r="I12" s="21">
-        <v>0.13</v>
+        <v>1.6E-2</v>
       </c>
       <c r="J12" s="20">
         <f t="shared" si="5"/>
-        <v>3.25</v>
+        <v>0.4</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="O12" s="44" t="s">
         <v>73</v>
-      </c>
-      <c r="M12" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="N12" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="O12" s="44" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25"/>
       <c r="C13" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -2663,112 +2843,170 @@
         <v>0.12</v>
       </c>
       <c r="G13" s="21">
-        <v>0.12</v>
+        <v>0.02</v>
       </c>
       <c r="H13" s="20">
         <f t="shared" si="3"/>
-        <v>1.2</v>
+        <v>0.2</v>
       </c>
       <c r="I13" s="21">
-        <v>0.12</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="J13" s="20">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="M13" s="29" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="O13" s="44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="38"/>
+      <c r="C14" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="38">
+        <v>0.12</v>
+      </c>
       <c r="F14" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="21"/>
+        <v>0.12</v>
+      </c>
+      <c r="G14" s="21">
+        <v>9.1999999999999998E-2</v>
+      </c>
       <c r="H14" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="21"/>
+        <v>0.91999999999999993</v>
+      </c>
+      <c r="I14" s="21">
+        <v>9.1999999999999998E-2</v>
+      </c>
       <c r="J14" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="44"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="M14" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="O14" s="44" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="38"/>
+      <c r="C15" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="38">
+        <v>0.12</v>
+      </c>
       <c r="F15" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="21"/>
+        <v>0.12</v>
+      </c>
+      <c r="G15" s="21">
+        <v>9.1999999999999998E-2</v>
+      </c>
       <c r="H15" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="21"/>
+        <v>0.91999999999999993</v>
+      </c>
+      <c r="I15" s="21">
+        <v>9.1999999999999998E-2</v>
+      </c>
       <c r="J15" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="44"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="O15" s="44" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="38"/>
+      <c r="C16" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="38">
+        <v>8.4499999999999993</v>
+      </c>
       <c r="F16" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="21"/>
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="G16" s="21">
+        <v>8.4499999999999993</v>
+      </c>
       <c r="H16" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="21"/>
+        <v>84.5</v>
+      </c>
+      <c r="I16" s="21">
+        <v>8.4499999999999993</v>
+      </c>
       <c r="J16" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="32"/>
+        <v>211.24999999999997</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" s="32" t="s">
+        <v>18</v>
+      </c>
       <c r="N16" s="27"/>
-      <c r="O16" s="44"/>
+      <c r="O16" s="44" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
@@ -3140,21 +3378,21 @@
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
-        <v>16.14</v>
+        <v>24.820000000000004</v>
       </c>
       <c r="G31" s="24" t="s">
         <v>15</v>
       </c>
       <c r="H31" s="24">
         <f>SUM(H4:H30)</f>
-        <v>155.35000000000002</v>
+        <v>239.58999999999997</v>
       </c>
       <c r="I31" s="24" t="s">
         <v>15</v>
       </c>
       <c r="J31" s="24">
         <f>SUM(J4:J30)</f>
-        <v>364.05</v>
+        <v>574.5</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -3163,21 +3401,21 @@
       </c>
       <c r="F32" s="24">
         <f>F31</f>
-        <v>16.14</v>
+        <v>24.820000000000004</v>
       </c>
       <c r="G32" t="s">
         <v>16</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
-        <v>15.535000000000002</v>
+        <v>23.958999999999996</v>
       </c>
       <c r="I32" t="s">
         <v>16</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
-        <v>14.562000000000001</v>
+        <v>22.98</v>
       </c>
     </row>
   </sheetData>
@@ -3196,18 +3434,15 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <ignoredErrors>
-    <ignoredError sqref="M12:M13" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3222,16 +3457,6 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>80</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added plotter code, BTEMS file name changing
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Full Instrument" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="130">
   <si>
     <t>Number</t>
   </si>
@@ -199,9 +202,6 @@
     <t>Comes in strips of 40, currently only need 34. Prices will be updated once precise count is established</t>
   </si>
   <si>
-    <t>Sensor Headers - Add to full instrument</t>
-  </si>
-  <si>
     <t>Red LED</t>
   </si>
   <si>
@@ -370,9 +370,6 @@
     <t>See 'Shield Parts'</t>
   </si>
   <si>
-    <t>Update male header requirements</t>
-  </si>
-  <si>
     <t>40-Pin 0.1" Breakaway Header</t>
   </si>
   <si>
@@ -385,9 +382,6 @@
     <t>https://www.sparkfun.com/products/553</t>
   </si>
   <si>
-    <t>Comes in strips of 40, currently only need 4/board. Actually used for SHT21 breakout</t>
-  </si>
-  <si>
     <t>Cost Percentage Breakdown</t>
   </si>
   <si>
@@ -422,6 +416,9 @@
   </si>
   <si>
     <t>Micro SD card but comes with standard size adapter</t>
+  </si>
+  <si>
+    <t>Comes in strips of 40, currently only need 4/board. Actually used for SHT21 breakout. Other sensor comes with headers</t>
   </si>
 </sst>
 </file>
@@ -1347,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1367,7 +1364,7 @@
     <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="119.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="76.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="98.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1412,7 +1409,7 @@
         <v>27</v>
       </c>
       <c r="P2" s="65" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q2" s="66"/>
       <c r="R2" s="67"/>
@@ -1431,19 +1428,19 @@
         <v>12</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" s="28" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>14</v>
@@ -1462,13 +1459,13 @@
       </c>
       <c r="O3" s="69"/>
       <c r="P3" s="55" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="Q3" s="56" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="R3" s="57" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -1650,10 +1647,10 @@
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>73</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>74</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -1680,7 +1677,7 @@
         <v>314</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L7" s="3">
         <v>3013</v>
@@ -1689,7 +1686,7 @@
         <v>30</v>
       </c>
       <c r="N7" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O7" s="44"/>
       <c r="P7" s="58">
@@ -1708,10 +1705,10 @@
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="25" t="s">
         <v>77</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>78</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -1738,19 +1735,19 @@
         <v>19.7</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="M8" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="M8" s="32" t="s">
+      <c r="N8" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="N8" s="19" t="s">
+      <c r="O8" s="44" t="s">
         <v>102</v>
-      </c>
-      <c r="O8" s="44" t="s">
-        <v>103</v>
       </c>
       <c r="P8" s="58">
         <f t="shared" si="3"/>
@@ -1768,7 +1765,7 @@
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>18</v>
@@ -1798,19 +1795,19 @@
         <v>45</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="N9" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="N9" s="19" t="s">
+      <c r="O9" s="44" t="s">
         <v>91</v>
-      </c>
-      <c r="O9" s="44" t="s">
-        <v>92</v>
       </c>
       <c r="P9" s="58">
         <f t="shared" si="3"/>
@@ -1828,7 +1825,7 @@
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>18</v>
@@ -1858,7 +1855,7 @@
         <v>17.8</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L10" s="3">
         <v>794</v>
@@ -1867,10 +1864,10 @@
         <v>18</v>
       </c>
       <c r="N10" s="19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="O10" s="44" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="P10" s="58">
         <f t="shared" si="3"/>
@@ -1888,7 +1885,7 @@
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>18</v>
@@ -1918,19 +1915,19 @@
         <v>59</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M11" s="32" t="s">
         <v>18</v>
       </c>
       <c r="N11" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="O11" s="44" t="s">
         <v>94</v>
-      </c>
-      <c r="O11" s="44" t="s">
-        <v>95</v>
       </c>
       <c r="P11" s="58">
         <f t="shared" si="3"/>
@@ -1948,7 +1945,7 @@
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>18</v>
@@ -1978,19 +1975,19 @@
         <v>62</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="N12" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="O12" s="44" t="s">
         <v>128</v>
-      </c>
-      <c r="M12" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="N12" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="O12" s="44" t="s">
-        <v>131</v>
       </c>
       <c r="P12" s="58">
         <f t="shared" si="3"/>
@@ -2008,7 +2005,7 @@
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>18</v>
@@ -2041,7 +2038,7 @@
         <v>574.5</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>18</v>
@@ -2051,7 +2048,7 @@
       </c>
       <c r="N13" s="19"/>
       <c r="O13" s="44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P13" s="58">
         <f t="shared" si="3"/>
@@ -2069,7 +2066,7 @@
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>18</v>
@@ -2102,16 +2099,16 @@
         <v>19</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M14" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="O14" s="44" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="P14" s="58">
         <f t="shared" si="3"/>
@@ -2891,19 +2888,19 @@
         <v>12</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" s="28" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>14</v>
@@ -3055,7 +3052,7 @@
         <v>26</v>
       </c>
       <c r="O6" s="44" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -3133,19 +3130,19 @@
         <v>8.9249999999999989</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M8" s="32" t="s">
         <v>18</v>
       </c>
       <c r="N8" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="O8" s="44" t="s">
         <v>80</v>
-      </c>
-      <c r="O8" s="44" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -3185,7 +3182,7 @@
         <v>54</v>
       </c>
       <c r="M9" s="32" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N9" s="19" t="s">
         <v>55</v>
@@ -3198,7 +3195,7 @@
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -3225,26 +3222,26 @@
         <v>1.9750000000000001</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="N10" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="N10" s="19" t="s">
-        <v>62</v>
-      </c>
       <c r="O10" s="44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -3271,26 +3268,26 @@
         <v>2.15</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="N11" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="M11" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>65</v>
-      </c>
       <c r="O11" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="34"/>
       <c r="C12" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -3317,26 +3314,26 @@
         <v>0.4</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M12" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O12" s="44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25"/>
       <c r="C13" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -3363,26 +3360,26 @@
         <v>0.44999999999999996</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M13" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O13" s="44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25"/>
       <c r="C14" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -3409,26 +3406,26 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M14" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O14" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -3455,26 +3452,26 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M15" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O15" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -3501,7 +3498,7 @@
         <v>211.24999999999997</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>18</v>
@@ -3511,7 +3508,7 @@
       </c>
       <c r="N16" s="27"/>
       <c r="O16" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -3945,10 +3942,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3958,16 +3955,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>114</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added radiation shield parts
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Full Instrument" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="145">
   <si>
     <t>Number</t>
   </si>
@@ -419,6 +419,51 @@
   </si>
   <si>
     <t>Comes in strips of 40, currently only need 4/board. Actually used for SHT21 breakout. Other sensor comes with headers</t>
+  </si>
+  <si>
+    <t>Radiation Shield</t>
+  </si>
+  <si>
+    <t>UofU MechE Dept.</t>
+  </si>
+  <si>
+    <t>Printed from UofU MechE 3D printer. Maybe cheaper elsewhere?</t>
+  </si>
+  <si>
+    <t>Set Screw</t>
+  </si>
+  <si>
+    <t>Quantity/Instrument</t>
+  </si>
+  <si>
+    <t>McMaster-Carr</t>
+  </si>
+  <si>
+    <t>91290A111</t>
+  </si>
+  <si>
+    <t>M3 0.5 x 6 Socket Head</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#91290A111</t>
+  </si>
+  <si>
+    <t>Comes in packs of 100 @ $7.78 per pack</t>
+  </si>
+  <si>
+    <t>Plasti-Dip White Spray</t>
+  </si>
+  <si>
+    <t>Home Depot</t>
+  </si>
+  <si>
+    <t>11 oz. Can</t>
+  </si>
+  <si>
+    <t>http://www.homedepot.com/p/Plasti-Dip-11-oz-White-General-Purpose-Rubber-Coating-Spray-11207-6/203286992</t>
+  </si>
+  <si>
+    <t>Assume 200 BTEMS can be made with one can</t>
   </si>
 </sst>
 </file>
@@ -1345,7 +1390,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1353,7 +1398,7 @@
     <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
@@ -1425,7 +1470,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>70</v>
@@ -1515,15 +1560,15 @@
       <c r="O4" s="43"/>
       <c r="P4" s="58">
         <f>F4/$F$31</f>
-        <v>8.6533981228782558E-2</v>
+        <v>8.0026889034715692E-2</v>
       </c>
       <c r="Q4" s="59">
         <f>H4/$H$31</f>
-        <v>8.9650226194416843E-2</v>
+        <v>8.2684892961225859E-2</v>
       </c>
       <c r="R4" s="60">
         <f>J4/$J$31</f>
-        <v>9.0890023072082785E-2</v>
+        <v>8.3738390960376288E-2</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -1575,15 +1620,15 @@
       </c>
       <c r="P5" s="58">
         <f t="shared" ref="P5:P30" si="3">F5/$F$31</f>
-        <v>0.14910470611728685</v>
+        <v>0.13789248572135626</v>
       </c>
       <c r="Q5" s="59">
         <f t="shared" ref="Q5:Q30" si="4">H5/$H$31</f>
-        <v>0.15447423590422596</v>
+        <v>0.14247243094857379</v>
       </c>
       <c r="R5" s="60">
         <f t="shared" ref="R5:R30" si="5">J5/$J$31</f>
-        <v>0.15661050129343496</v>
+        <v>0.1442876890394176</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -1633,15 +1678,15 @@
       <c r="O6" s="44"/>
       <c r="P6" s="58">
         <f t="shared" si="3"/>
-        <v>0.13246355588098252</v>
+        <v>0.12250269936852631</v>
       </c>
       <c r="Q6" s="59">
         <f t="shared" si="4"/>
-        <v>0.13723380778991504</v>
+        <v>0.12657148999449191</v>
       </c>
       <c r="R6" s="60">
         <f t="shared" si="5"/>
-        <v>0.13913165070264977</v>
+        <v>0.12818415231626831</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -1679,7 +1724,7 @@
       <c r="K7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="29">
         <v>3013</v>
       </c>
       <c r="M7" s="32" t="s">
@@ -1691,15 +1736,15 @@
       <c r="O7" s="44"/>
       <c r="P7" s="58">
         <f t="shared" si="3"/>
-        <v>0.18571523663715639</v>
+        <v>0.17175001569758214</v>
       </c>
       <c r="Q7" s="59">
         <f t="shared" si="4"/>
-        <v>0.17323182169259627</v>
+        <v>0.15977265470661492</v>
       </c>
       <c r="R7" s="60">
         <f t="shared" si="5"/>
-        <v>0.17562749073620917</v>
+        <v>0.16180833699420402</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -1751,15 +1796,15 @@
       </c>
       <c r="P8" s="58">
         <f t="shared" si="3"/>
-        <v>1.1582240564467819E-2</v>
+        <v>1.0711291301569639E-2</v>
       </c>
       <c r="Q8" s="59">
         <f t="shared" si="4"/>
-        <v>1.0868365883261613E-2</v>
+        <v>1.002395317745323E-2</v>
       </c>
       <c r="R8" s="60">
         <f t="shared" si="5"/>
-        <v>1.1018667412430959E-2</v>
+        <v>1.015166955027331E-2</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -1811,15 +1856,15 @@
       </c>
       <c r="P9" s="58">
         <f t="shared" si="3"/>
-        <v>2.3963256340278245E-2</v>
+        <v>2.2161292348075113E-2</v>
       </c>
       <c r="Q9" s="59">
         <f t="shared" si="4"/>
-        <v>2.4826216484607744E-2</v>
+        <v>2.2897354973877931E-2</v>
       </c>
       <c r="R9" s="60">
         <f t="shared" si="5"/>
-        <v>2.5169544850730616E-2</v>
+        <v>2.3189092881334972E-2</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -1857,7 +1902,7 @@
       <c r="K10" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="29">
         <v>794</v>
       </c>
       <c r="M10" s="32" t="s">
@@ -1871,15 +1916,15 @@
       </c>
       <c r="P10" s="58">
         <f t="shared" si="3"/>
-        <v>1.0517206949344342E-2</v>
+        <v>9.7263449749885218E-3</v>
       </c>
       <c r="Q10" s="59">
         <f t="shared" si="4"/>
-        <v>9.8201478539115088E-3</v>
+        <v>9.0571759674450501E-3</v>
       </c>
       <c r="R10" s="60">
         <f t="shared" si="5"/>
-        <v>9.9559532965112219E-3</v>
+        <v>9.1725745175058344E-3</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -1931,15 +1976,15 @@
       </c>
       <c r="P11" s="58">
         <f t="shared" si="3"/>
-        <v>3.4081075683951287E-2</v>
+        <v>3.1518282450595715E-2</v>
       </c>
       <c r="Q11" s="59">
         <f t="shared" si="4"/>
-        <v>3.2549928279819035E-2</v>
+        <v>3.0020976521306621E-2</v>
       </c>
       <c r="R11" s="60">
         <f t="shared" si="5"/>
-        <v>3.3000069915402365E-2</v>
+        <v>3.0403477333305853E-2</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -1991,15 +2036,15 @@
       </c>
       <c r="P12" s="58">
         <f t="shared" si="3"/>
-        <v>3.3016042068827807E-2</v>
+        <v>3.0533336124014602E-2</v>
       </c>
       <c r="Q12" s="59">
         <f t="shared" si="4"/>
-        <v>3.4205009378792894E-2</v>
+        <v>3.1547466852898484E-2</v>
       </c>
       <c r="R12" s="60">
         <f t="shared" si="5"/>
-        <v>3.4678039572117736E-2</v>
+        <v>3.194941685872818E-2</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -2052,15 +2097,15 @@
       </c>
       <c r="P13" s="58">
         <f t="shared" si="3"/>
-        <v>0.33042667909205897</v>
+        <v>0.30557959782179134</v>
       </c>
       <c r="Q13" s="59">
         <f t="shared" si="4"/>
-        <v>0.33045073375262046</v>
+        <v>0.3047765154550785</v>
       </c>
       <c r="R13" s="60">
         <f t="shared" si="5"/>
-        <v>0.32133118926099419</v>
+        <v>0.29604741911837645</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -2112,129 +2157,194 @@
       </c>
       <c r="P14" s="58">
         <f t="shared" si="3"/>
-        <v>2.5960194368634766E-3</v>
+        <v>2.4008066710414708E-3</v>
       </c>
       <c r="Q14" s="59">
         <f t="shared" si="4"/>
-        <v>2.6895067858325058E-3</v>
+        <v>2.480546788836776E-3</v>
       </c>
       <c r="R14" s="60">
         <f t="shared" si="5"/>
-        <v>2.5868698874362025E-3</v>
+        <v>2.3833234350260947E-3</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="38"/>
+      <c r="B15" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="38">
+        <v>6</v>
+      </c>
       <c r="F15" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="21"/>
+        <v>6</v>
+      </c>
+      <c r="G15" s="21">
+        <v>6</v>
+      </c>
       <c r="H15" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="21"/>
+        <v>60</v>
+      </c>
+      <c r="I15" s="21">
+        <v>6</v>
+      </c>
       <c r="J15" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="29"/>
+        <v>150</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L15" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>18</v>
+      </c>
       <c r="N15" s="19"/>
-      <c r="O15" s="44"/>
+      <c r="O15" s="44" t="s">
+        <v>132</v>
+      </c>
       <c r="P15" s="58">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7.3870974493583708E-2</v>
       </c>
       <c r="Q15" s="59">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7.6324516579593105E-2</v>
       </c>
       <c r="R15" s="60">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7.7296976271116577E-2</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="38"/>
+      <c r="B16" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="38">
+        <v>7.7799999999999994E-2</v>
+      </c>
       <c r="F16" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="21"/>
+        <v>7.7799999999999994E-2</v>
+      </c>
+      <c r="G16" s="21">
+        <v>7.7799999999999994E-2</v>
+      </c>
       <c r="H16" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="21"/>
+        <v>0.77799999999999991</v>
+      </c>
+      <c r="I16" s="21">
+        <v>7.7799999999999994E-2</v>
+      </c>
       <c r="J16" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="44"/>
+        <v>1.9449999999999998</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="M16" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="N16" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="O16" s="44" t="s">
+        <v>139</v>
+      </c>
       <c r="P16" s="58">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>9.5786030260013543E-4</v>
       </c>
       <c r="Q16" s="59">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>9.8967456498205708E-4</v>
       </c>
       <c r="R16" s="60">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.0022841256488114E-3</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="38"/>
+      <c r="B17" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="4">
+        <f>1/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E17" s="38">
+        <v>5.98</v>
+      </c>
       <c r="F17" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="21"/>
+        <v>2.9900000000000003E-2</v>
+      </c>
+      <c r="G17" s="21">
+        <v>5.98</v>
+      </c>
       <c r="H17" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="21"/>
+        <v>0.29900000000000004</v>
+      </c>
+      <c r="I17" s="21">
+        <v>5.98</v>
+      </c>
       <c r="J17" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="44"/>
+        <v>0.74750000000000005</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L17" s="29">
+        <v>203286992</v>
+      </c>
+      <c r="M17" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="N17" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="O17" s="44" t="s">
+        <v>144</v>
+      </c>
       <c r="P17" s="58">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.6812368955969221E-4</v>
       </c>
       <c r="Q17" s="59">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.8035050762163906E-4</v>
       </c>
       <c r="R17" s="60">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.8519659841773093E-4</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -2737,26 +2847,26 @@
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
-        <v>75.114999999999981</v>
+        <v>81.222699999999975</v>
       </c>
       <c r="G31" s="24" t="s">
         <v>15</v>
       </c>
       <c r="H31" s="24">
         <f>SUM(H4:H30)</f>
-        <v>725.04000000000008</v>
+        <v>786.11700000000008</v>
       </c>
       <c r="I31" s="24" t="s">
         <v>15</v>
       </c>
       <c r="J31" s="24">
         <f>SUM(J4:J30)</f>
-        <v>1787.875</v>
+        <v>1940.5674999999999</v>
       </c>
       <c r="M31" s="30"/>
       <c r="P31" s="64">
         <f>SUM(P4:P30)</f>
-        <v>1.0000000000000002</v>
+        <v>1.0000000000000004</v>
       </c>
       <c r="Q31" s="64">
         <f t="shared" ref="Q31:R31" si="9">SUM(Q4:Q30)</f>
@@ -2764,7 +2874,7 @@
       </c>
       <c r="R31" s="64">
         <f t="shared" si="9"/>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
@@ -2773,21 +2883,21 @@
       </c>
       <c r="F32" s="24">
         <f>F31</f>
-        <v>75.114999999999981</v>
+        <v>81.222699999999975</v>
       </c>
       <c r="G32" t="s">
         <v>16</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
-        <v>72.504000000000005</v>
+        <v>78.611700000000013</v>
       </c>
       <c r="I32" t="s">
         <v>16</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
-        <v>71.515000000000001</v>
+        <v>77.622699999999995</v>
       </c>
       <c r="M32" s="30"/>
     </row>

</xml_diff>

<commit_message>
Added schematic names to BOM
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27211"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27217"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Full Instrument" sheetId="3" r:id="rId1"/>
@@ -29,14 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="155">
   <si>
     <t>Number</t>
   </si>
   <si>
-    <t>Schematic Name</t>
-  </si>
-  <si>
     <t>Part Name</t>
   </si>
   <si>
@@ -464,6 +461,39 @@
   </si>
   <si>
     <t>MLX90614</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>SDSLOT</t>
+  </si>
+  <si>
+    <t>RTC_HEADER</t>
+  </si>
+  <si>
+    <t>BAT_HEADER</t>
+  </si>
+  <si>
+    <t>RED_LED</t>
+  </si>
+  <si>
+    <t>GREEN_LED</t>
+  </si>
+  <si>
+    <t>R_RLED</t>
+  </si>
+  <si>
+    <t>R_GLED</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>EAGLE Schematic Name</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1414,47 +1444,47 @@
   <sheetData>
     <row r="1" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="71"/>
       <c r="C1" s="1">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="73"/>
       <c r="C2" s="74"/>
       <c r="D2" s="17"/>
       <c r="E2" s="72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="75"/>
       <c r="G2" s="76" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="75"/>
       <c r="I2" s="72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2" s="75"/>
       <c r="K2" s="72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L2" s="73"/>
       <c r="M2" s="74"/>
       <c r="N2" s="75"/>
       <c r="O2" s="68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P2" s="65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q2" s="66"/>
       <c r="R2" s="67"/>
@@ -1464,62 +1494,62 @@
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="M3" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="13" t="s">
         <v>4</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>5</v>
       </c>
       <c r="O3" s="69"/>
       <c r="P3" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q3" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="Q3" s="56" t="s">
+      <c r="R3" s="57" t="s">
         <v>118</v>
-      </c>
-      <c r="R3" s="57" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -1546,16 +1576,16 @@
         <v>162.5</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="M4" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="M4" s="29" t="s">
+      <c r="N4" s="19" t="s">
         <v>29</v>
-      </c>
-      <c r="N4" s="19" t="s">
-        <v>30</v>
       </c>
       <c r="O4" s="43"/>
       <c r="P4" s="58">
@@ -1574,10 +1604,10 @@
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1604,19 +1634,19 @@
         <v>280</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="19" t="s">
+      <c r="O5" s="44" t="s">
         <v>50</v>
-      </c>
-      <c r="O5" s="44" t="s">
-        <v>51</v>
       </c>
       <c r="P5" s="58">
         <f t="shared" ref="P5:P30" si="3">F5/$F$31</f>
@@ -1634,10 +1664,10 @@
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -1664,16 +1694,16 @@
         <v>248.74999999999997</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="27" t="s">
         <v>37</v>
-      </c>
-      <c r="M6" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" s="27" t="s">
-        <v>38</v>
       </c>
       <c r="O6" s="44"/>
       <c r="P6" s="58">
@@ -1692,10 +1722,10 @@
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -1722,16 +1752,16 @@
         <v>314</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L7" s="29">
         <v>3013</v>
       </c>
       <c r="M7" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N7" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O7" s="44"/>
       <c r="P7" s="58">
@@ -1750,10 +1780,10 @@
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="25" t="s">
         <v>75</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>76</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -1780,19 +1810,19 @@
         <v>19.7</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M8" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="M8" s="32" t="s">
+      <c r="N8" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="N8" s="19" t="s">
+      <c r="O8" s="44" t="s">
         <v>100</v>
-      </c>
-      <c r="O8" s="44" t="s">
-        <v>101</v>
       </c>
       <c r="P8" s="58">
         <f t="shared" si="3"/>
@@ -1810,10 +1840,10 @@
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="4">
         <v>8</v>
@@ -1840,19 +1870,19 @@
         <v>45</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="M9" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="N9" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="N9" s="19" t="s">
+      <c r="O9" s="44" t="s">
         <v>89</v>
-      </c>
-      <c r="O9" s="44" t="s">
-        <v>90</v>
       </c>
       <c r="P9" s="58">
         <f t="shared" si="3"/>
@@ -1870,10 +1900,10 @@
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="4">
         <v>0.2</v>
@@ -1900,19 +1930,19 @@
         <v>17.8</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L10" s="29">
         <v>794</v>
       </c>
       <c r="M10" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N10" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="O10" s="44" t="s">
         <v>121</v>
-      </c>
-      <c r="O10" s="44" t="s">
-        <v>122</v>
       </c>
       <c r="P10" s="58">
         <f t="shared" si="3"/>
@@ -1930,10 +1960,10 @@
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4">
         <v>2</v>
@@ -1960,19 +1990,19 @@
         <v>59</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="M11" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="N11" s="19" t="s">
+      <c r="O11" s="44" t="s">
         <v>92</v>
-      </c>
-      <c r="O11" s="44" t="s">
-        <v>93</v>
       </c>
       <c r="P11" s="58">
         <f t="shared" si="3"/>
@@ -1990,10 +2020,10 @@
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -2020,19 +2050,19 @@
         <v>62</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="M12" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="M12" s="29" t="s">
+      <c r="N12" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="N12" s="19" t="s">
+      <c r="O12" s="44" t="s">
         <v>126</v>
-      </c>
-      <c r="O12" s="44" t="s">
-        <v>127</v>
       </c>
       <c r="P12" s="58">
         <f t="shared" si="3"/>
@@ -2050,10 +2080,10 @@
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -2083,17 +2113,17 @@
         <v>574.5</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M13" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N13" s="19"/>
       <c r="O13" s="44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P13" s="58">
         <f t="shared" si="3"/>
@@ -2111,10 +2141,10 @@
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" s="4">
         <v>0.1</v>
@@ -2141,19 +2171,19 @@
         <v>4.6250000000000009</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L14" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M14" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="M14" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" s="19" t="s">
-        <v>115</v>
-      </c>
       <c r="O14" s="44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P14" s="58">
         <f t="shared" si="3"/>
@@ -2171,10 +2201,10 @@
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -2201,17 +2231,17 @@
         <v>150</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L15" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M15" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N15" s="19"/>
       <c r="O15" s="44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P15" s="58">
         <f t="shared" si="3"/>
@@ -2229,10 +2259,10 @@
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -2259,19 +2289,19 @@
         <v>1.9449999999999998</v>
       </c>
       <c r="K16" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="M16" s="32" t="s">
+      <c r="N16" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="N16" s="27" t="s">
+      <c r="O16" s="44" t="s">
         <v>137</v>
-      </c>
-      <c r="O16" s="44" t="s">
-        <v>138</v>
       </c>
       <c r="P16" s="58">
         <f t="shared" si="3"/>
@@ -2289,10 +2319,10 @@
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="4">
         <f>1/200</f>
@@ -2320,19 +2350,19 @@
         <v>0.74750000000000005</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L17" s="29">
         <v>203286992</v>
       </c>
       <c r="M17" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="N17" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="N17" s="19" t="s">
+      <c r="O17" s="44" t="s">
         <v>142</v>
-      </c>
-      <c r="O17" s="44" t="s">
-        <v>143</v>
       </c>
       <c r="P17" s="58">
         <f t="shared" si="3"/>
@@ -2843,21 +2873,21 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E31" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
         <v>81.222699999999975</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" s="24">
         <f>SUM(H4:H30)</f>
         <v>786.11700000000008</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J31" s="24">
         <f>SUM(J4:J30)</f>
@@ -2879,21 +2909,21 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F32" s="24">
         <f>F31</f>
         <v>81.222699999999975</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
         <v>78.611700000000013</v>
       </c>
       <c r="I32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
@@ -2920,14 +2950,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
@@ -2945,43 +2975,43 @@
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="71"/>
       <c r="C1" s="1">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="73"/>
       <c r="C2" s="74"/>
       <c r="D2" s="17"/>
       <c r="E2" s="72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="75"/>
       <c r="G2" s="76" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="75"/>
       <c r="I2" s="72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2" s="75"/>
       <c r="K2" s="72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L2" s="73"/>
       <c r="M2" s="74"/>
       <c r="N2" s="75"/>
       <c r="O2" s="77" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2989,51 +3019,53 @@
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="L3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="14" t="s">
+      <c r="N3" s="13" t="s">
         <v>4</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>5</v>
       </c>
       <c r="O3" s="78"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="C4" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -3060,26 +3092,28 @@
         <v>224.00000000000003</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="19" t="s">
+      <c r="O4" s="43" t="s">
         <v>47</v>
-      </c>
-      <c r="O4" s="43" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="25"/>
+      <c r="B5" s="25" t="s">
+        <v>144</v>
+      </c>
       <c r="C5" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -3106,24 +3140,26 @@
         <v>35.75</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="19" t="s">
         <v>21</v>
-      </c>
-      <c r="M5" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>22</v>
       </c>
       <c r="O5" s="44"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
-      <c r="B6" s="25"/>
+      <c r="B6" s="25" t="s">
+        <v>145</v>
+      </c>
       <c r="C6" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -3150,26 +3186,28 @@
         <v>37.25</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" s="27" t="s">
-        <v>26</v>
-      </c>
       <c r="O6" s="44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
+      <c r="B7" s="25" t="s">
+        <v>146</v>
+      </c>
       <c r="C7" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -3196,24 +3234,26 @@
         <v>12</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="32" t="s">
+      <c r="N7" s="19" t="s">
         <v>41</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>42</v>
       </c>
       <c r="O7" s="44"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="25"/>
+      <c r="B8" s="25" t="s">
+        <v>147</v>
+      </c>
       <c r="C8" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -3240,26 +3280,28 @@
         <v>8.9249999999999989</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="M8" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="N8" s="19" t="s">
+      <c r="O8" s="44" t="s">
         <v>78</v>
-      </c>
-      <c r="O8" s="44" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
+      <c r="B9" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -3286,26 +3328,28 @@
         <v>35.75</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L9" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="N9" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="N9" s="19" t="s">
+      <c r="O9" s="44" t="s">
         <v>54</v>
-      </c>
-      <c r="O9" s="44" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
+      <c r="B10" s="25" t="s">
+        <v>148</v>
+      </c>
       <c r="C10" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -3332,26 +3376,28 @@
         <v>1.9750000000000001</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="N10" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="N10" s="19" t="s">
-        <v>60</v>
-      </c>
       <c r="O10" s="44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="25"/>
+      <c r="B11" s="25" t="s">
+        <v>149</v>
+      </c>
       <c r="C11" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -3378,26 +3424,28 @@
         <v>2.15</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="N11" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="M11" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>63</v>
-      </c>
       <c r="O11" s="44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="34"/>
+      <c r="B12" s="34" t="s">
+        <v>150</v>
+      </c>
       <c r="C12" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -3424,26 +3472,28 @@
         <v>0.4</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L12" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="M12" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="N12" s="19" t="s">
-        <v>103</v>
-      </c>
       <c r="O12" s="44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="25"/>
+      <c r="B13" s="25" t="s">
+        <v>151</v>
+      </c>
       <c r="C13" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -3470,26 +3520,28 @@
         <v>0.44999999999999996</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L13" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="M13" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="M13" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="N13" s="19" t="s">
-        <v>105</v>
-      </c>
       <c r="O13" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="25"/>
+      <c r="B14" s="25" t="s">
+        <v>152</v>
+      </c>
       <c r="C14" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -3516,26 +3568,28 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L14" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M14" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="M14" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" s="19" t="s">
-        <v>107</v>
-      </c>
       <c r="O14" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="25"/>
+      <c r="B15" s="25" t="s">
+        <v>153</v>
+      </c>
       <c r="C15" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -3562,26 +3616,28 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="N15" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="M15" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="N15" s="19" t="s">
-        <v>109</v>
-      </c>
       <c r="O15" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="25"/>
+      <c r="B16" s="25" t="s">
+        <v>17</v>
+      </c>
       <c r="C16" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -3608,17 +3664,17 @@
         <v>211.24999999999997</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M16" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N16" s="27"/>
       <c r="O16" s="44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -3987,21 +4043,21 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E31" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
         <v>24.820000000000004</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" s="24">
         <f>SUM(H4:H30)</f>
         <v>239.58999999999997</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J31" s="24">
         <f>SUM(J4:J30)</f>
@@ -4010,21 +4066,21 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F32" s="24">
         <f>F31</f>
         <v>24.820000000000004</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
         <v>23.958999999999996</v>
       </c>
       <c r="I32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
@@ -4062,7 +4118,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added info for 6-22-16 order
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Full Instrument" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="161">
   <si>
     <t>Number</t>
   </si>
@@ -334,12 +334,6 @@
     <t>Much cheaper if bought in quantities of 50+</t>
   </si>
   <si>
-    <t>588-OK2715E-R52</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Ohmite/OK2715E-R52/?qs=sGAEpiMZZMtlubZbdhIBIJMLE6vvLglcKmeAomrNvK0%3d</t>
-  </si>
-  <si>
     <t>588-OK2215E-R52</t>
   </si>
   <si>
@@ -400,18 +394,9 @@
     <t>Newegg</t>
   </si>
   <si>
-    <t>9SIA6NC35M9501</t>
-  </si>
-  <si>
     <t>Micro SD with Regular Adapter</t>
   </si>
   <si>
-    <t>http://www.newegg.com/Product/Product.aspx?Item=9SIA6NC35M9501&amp;cm_re=sd_card-_-20-134-717-_-Product</t>
-  </si>
-  <si>
-    <t>Micro SD card but comes with standard size adapter</t>
-  </si>
-  <si>
     <t>Comes in strips of 40, currently only need 4/board. Actually used for SHT21 breakout. Other sensor comes with headers</t>
   </si>
   <si>
@@ -494,6 +479,39 @@
   </si>
   <si>
     <t>EAGLE Schematic Name</t>
+  </si>
+  <si>
+    <t>6/22/2016 Order</t>
+  </si>
+  <si>
+    <t>Quantity Ordered</t>
+  </si>
+  <si>
+    <t>Cost/Unit</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>BTEMS Required:</t>
+  </si>
+  <si>
+    <t>9SIA1EK0HR9980</t>
+  </si>
+  <si>
+    <t>http://www.newegg.com/Product/Product.aspx?Item=9SIA1EK0HR9980</t>
+  </si>
+  <si>
+    <t>Total Order Cost:</t>
+  </si>
+  <si>
+    <t>Micro SD card but comes with standard size adapter - Not reliable source</t>
+  </si>
+  <si>
+    <t>279-CFR25J270R</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/TE-Connectivity-Neohm/CFR25J270R/?qs=sGAEpiMZZMu61qfTUdNhG05q5R9Z8%252b9s90AksAri%2fIw%3d</t>
   </si>
 </sst>
 </file>
@@ -505,7 +523,14 @@
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -546,7 +571,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -925,30 +950,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -970,7 +1026,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="17" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -978,7 +1034,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="17" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
@@ -995,7 +1051,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
@@ -1062,8 +1118,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="20" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="20" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="26" xfId="20" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="21">
+    <cellStyle name="Currency" xfId="20" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1417,10 +1484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1440,9 +1507,11 @@
     <col min="13" max="13" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="119.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="98.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>10</v>
       </c>
@@ -1454,8 +1523,14 @@
         <v>44</v>
       </c>
       <c r="M1" s="30"/>
-    </row>
-    <row r="2" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>154</v>
+      </c>
+      <c r="T1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
         <v>6</v>
       </c>
@@ -1484,12 +1559,17 @@
         <v>26</v>
       </c>
       <c r="P2" s="65" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Q2" s="66"/>
       <c r="R2" s="67"/>
-    </row>
-    <row r="3" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S2" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="T2" s="66"/>
+      <c r="U2" s="67"/>
+    </row>
+    <row r="3" spans="1:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -1500,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>68</v>
@@ -1534,22 +1614,31 @@
       </c>
       <c r="O3" s="69"/>
       <c r="P3" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q3" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="R3" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="Q3" s="56" t="s">
-        <v>117</v>
-      </c>
-      <c r="R3" s="57" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S3" s="80" t="s">
+        <v>151</v>
+      </c>
+      <c r="T3" s="81" t="s">
+        <v>152</v>
+      </c>
+      <c r="U3" s="79" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -1579,7 +1668,7 @@
         <v>27</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="M4" s="29" t="s">
         <v>28</v>
@@ -1590,18 +1679,30 @@
       <c r="O4" s="43"/>
       <c r="P4" s="58">
         <f>F4/$F$31</f>
-        <v>8.0026889034715692E-2</v>
+        <v>7.9015155106749502E-2</v>
       </c>
       <c r="Q4" s="59">
         <f>H4/$H$31</f>
-        <v>8.2684892961225859E-2</v>
+        <v>8.1555118085537517E-2</v>
       </c>
       <c r="R4" s="60">
         <f>J4/$J$31</f>
-        <v>8.3738390960376288E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+        <v>8.2314219971455965E-2</v>
+      </c>
+      <c r="S4" s="2">
+        <f>$T$1*D4</f>
+        <v>58</v>
+      </c>
+      <c r="T4" s="82">
+        <f>E4</f>
+        <v>6.5</v>
+      </c>
+      <c r="U4" s="84">
+        <f>S4*T4</f>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="25" t="s">
         <v>32</v>
@@ -1650,18 +1751,30 @@
       </c>
       <c r="P5" s="58">
         <f t="shared" ref="P5:P30" si="3">F5/$F$31</f>
-        <v>0.13789248572135626</v>
+        <v>0.13614919033778375</v>
       </c>
       <c r="Q5" s="59">
         <f t="shared" ref="Q5:Q30" si="4">H5/$H$31</f>
-        <v>0.14247243094857379</v>
+        <v>0.1405257419320031</v>
       </c>
       <c r="R5" s="60">
         <f t="shared" ref="R5:R30" si="5">J5/$J$31</f>
-        <v>0.1442876890394176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+        <v>0.14183373287389336</v>
+      </c>
+      <c r="S5" s="2">
+        <f t="shared" ref="S5:S30" si="6">$T$1*D5</f>
+        <v>58</v>
+      </c>
+      <c r="T5" s="82">
+        <f>E5</f>
+        <v>11.2</v>
+      </c>
+      <c r="U5" s="84">
+        <f t="shared" ref="U5:U30" si="7">S5*T5</f>
+        <v>649.59999999999991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
         <v>34</v>
@@ -1673,25 +1786,25 @@
         <v>1</v>
       </c>
       <c r="E6" s="38">
-        <v>9.9499999999999993</v>
+        <v>10.5</v>
       </c>
       <c r="F6" s="26">
         <f t="shared" si="0"/>
-        <v>9.9499999999999993</v>
+        <v>10.5</v>
       </c>
       <c r="G6" s="21">
-        <v>9.9499999999999993</v>
+        <v>10.5</v>
       </c>
       <c r="H6" s="20">
         <f t="shared" si="1"/>
-        <v>99.5</v>
+        <v>105</v>
       </c>
       <c r="I6" s="21">
-        <v>9.9499999999999993</v>
+        <v>10.5</v>
       </c>
       <c r="J6" s="20">
         <f t="shared" si="2"/>
-        <v>248.74999999999997</v>
+        <v>262.5</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>35</v>
@@ -1708,18 +1821,30 @@
       <c r="O6" s="44"/>
       <c r="P6" s="58">
         <f t="shared" si="3"/>
-        <v>0.12250269936852631</v>
+        <v>0.12763986594167229</v>
       </c>
       <c r="Q6" s="59">
         <f t="shared" si="4"/>
-        <v>0.12657148999449191</v>
+        <v>0.1317428830612529</v>
       </c>
       <c r="R6" s="60">
         <f t="shared" si="5"/>
-        <v>0.12818415231626831</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+        <v>0.13296912456927501</v>
+      </c>
+      <c r="S6" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T6" s="82">
+        <f>E6</f>
+        <v>10.5</v>
+      </c>
+      <c r="U6" s="84">
+        <f t="shared" si="7"/>
+        <v>609</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
         <v>70</v>
@@ -1766,18 +1891,30 @@
       <c r="O7" s="44"/>
       <c r="P7" s="58">
         <f t="shared" si="3"/>
-        <v>0.17175001569758214</v>
+        <v>0.16957867903679316</v>
       </c>
       <c r="Q7" s="59">
         <f t="shared" si="4"/>
-        <v>0.15977265470661492</v>
+        <v>0.15758958202374634</v>
       </c>
       <c r="R7" s="60">
         <f t="shared" si="5"/>
-        <v>0.16180833699420402</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+        <v>0.15905640043715183</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T7" s="82">
+        <f>G7</f>
+        <v>12.56</v>
+      </c>
+      <c r="U7" s="84">
+        <f t="shared" si="7"/>
+        <v>728.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
         <v>74</v>
@@ -1826,18 +1963,29 @@
       </c>
       <c r="P8" s="58">
         <f t="shared" si="3"/>
-        <v>1.0711291301569639E-2</v>
+        <v>1.0575874606595703E-2</v>
       </c>
       <c r="Q8" s="59">
         <f t="shared" si="4"/>
-        <v>1.002395317745323E-2</v>
+        <v>9.8869897002159327E-3</v>
       </c>
       <c r="R8" s="60">
         <f t="shared" si="5"/>
-        <v>1.015166955027331E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+        <v>9.9790162057703542E-3</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T8" s="82">
+        <v>0.7</v>
+      </c>
+      <c r="U8" s="84">
+        <f t="shared" si="7"/>
+        <v>40.599999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="25" t="s">
         <v>79</v>
@@ -1886,18 +2034,28 @@
       </c>
       <c r="P9" s="58">
         <f t="shared" si="3"/>
-        <v>2.2161292348075113E-2</v>
+        <v>2.1881119875715248E-2</v>
       </c>
       <c r="Q9" s="59">
         <f t="shared" si="4"/>
-        <v>2.2897354973877931E-2</v>
+        <v>2.2584494239071926E-2</v>
       </c>
       <c r="R9" s="60">
         <f t="shared" si="5"/>
-        <v>2.3189092881334972E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+        <v>2.2794707069018576E-2</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0</v>
+      </c>
+      <c r="T9" s="82">
+        <v>0.23</v>
+      </c>
+      <c r="U9" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
         <v>85</v>
@@ -1939,28 +2097,39 @@
         <v>17</v>
       </c>
       <c r="N10" s="19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="O10" s="44" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="P10" s="58">
         <f t="shared" si="3"/>
-        <v>9.7263449749885218E-3</v>
+        <v>9.6033803898972481E-3</v>
       </c>
       <c r="Q10" s="59">
         <f t="shared" si="4"/>
-        <v>9.0571759674450501E-3</v>
+        <v>8.9334221656773415E-3</v>
       </c>
       <c r="R10" s="60">
         <f t="shared" si="5"/>
-        <v>9.1725745175058344E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+        <v>9.0165730184117929E-3</v>
+      </c>
+      <c r="S10" s="2">
+        <v>12</v>
+      </c>
+      <c r="T10" s="82">
+        <f>G10</f>
+        <v>3.56</v>
+      </c>
+      <c r="U10" s="84">
+        <f t="shared" si="7"/>
+        <v>42.72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>17</v>
@@ -1969,25 +2138,25 @@
         <v>2</v>
       </c>
       <c r="E11" s="38">
-        <v>1.28</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="F11" s="26">
         <f t="shared" si="0"/>
-        <v>2.56</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G11" s="21">
-        <v>1.18</v>
+        <v>1.06</v>
       </c>
       <c r="H11" s="20">
         <f t="shared" si="1"/>
-        <v>23.599999999999998</v>
+        <v>21.200000000000003</v>
       </c>
       <c r="I11" s="21">
-        <v>1.18</v>
+        <v>1.06</v>
       </c>
       <c r="J11" s="20">
         <f t="shared" si="2"/>
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>56</v>
@@ -2006,18 +2175,29 @@
       </c>
       <c r="P11" s="58">
         <f t="shared" si="3"/>
-        <v>3.1518282450595715E-2</v>
+        <v>2.7959208730080592E-2</v>
       </c>
       <c r="Q11" s="59">
         <f t="shared" si="4"/>
-        <v>3.0020976521306621E-2</v>
+        <v>2.659951543712916E-2</v>
       </c>
       <c r="R11" s="60">
         <f t="shared" si="5"/>
-        <v>3.0403477333305853E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+        <v>2.6847099436844098E-2</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="6"/>
+        <v>116</v>
+      </c>
+      <c r="T11" s="82">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="U11" s="84">
+        <f t="shared" si="7"/>
+        <v>104.864</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="34" t="s">
         <v>93</v>
@@ -2029,55 +2209,67 @@
         <v>1</v>
       </c>
       <c r="E12" s="38">
-        <v>2.48</v>
+        <v>3.6</v>
       </c>
       <c r="F12" s="26">
         <f t="shared" si="0"/>
-        <v>2.48</v>
+        <v>3.6</v>
       </c>
       <c r="G12" s="21">
-        <v>2.48</v>
+        <v>3.6</v>
       </c>
       <c r="H12" s="20">
         <f t="shared" si="1"/>
-        <v>24.8</v>
+        <v>36</v>
       </c>
       <c r="I12" s="21">
-        <v>2.48</v>
+        <v>3.6</v>
       </c>
       <c r="J12" s="20">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="M12" s="29" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="O12" s="44" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="P12" s="58">
         <f t="shared" si="3"/>
-        <v>3.0533336124014602E-2</v>
+        <v>4.3762239751430496E-2</v>
       </c>
       <c r="Q12" s="59">
         <f t="shared" si="4"/>
-        <v>3.1547466852898484E-2</v>
+        <v>4.5168988478143851E-2</v>
       </c>
       <c r="R12" s="60">
         <f t="shared" si="5"/>
-        <v>3.194941685872818E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+        <v>4.5589414138037153E-2</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T12" s="82">
+        <f>E12</f>
+        <v>3.6</v>
+      </c>
+      <c r="U12" s="84">
+        <f t="shared" si="7"/>
+        <v>208.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25" t="s">
         <v>94</v>
@@ -2090,30 +2282,30 @@
       </c>
       <c r="E13" s="38">
         <f>'Shield Parts'!$F$32</f>
-        <v>24.820000000000004</v>
+        <v>24.449999999999996</v>
       </c>
       <c r="F13" s="26">
-        <f t="shared" ref="F13" si="6">D13*E13</f>
-        <v>24.820000000000004</v>
+        <f t="shared" ref="F13" si="8">D13*E13</f>
+        <v>24.449999999999996</v>
       </c>
       <c r="G13" s="21">
         <f>'Shield Parts'!$H$32</f>
-        <v>23.958999999999996</v>
+        <v>23.617999999999999</v>
       </c>
       <c r="H13" s="20">
-        <f t="shared" ref="H13" si="7">G13*D13*10</f>
-        <v>239.58999999999997</v>
+        <f t="shared" ref="H13" si="9">G13*D13*10</f>
+        <v>236.17999999999998</v>
       </c>
       <c r="I13" s="21">
         <f>'Shield Parts'!$J$32</f>
-        <v>22.98</v>
+        <v>22.893000000000001</v>
       </c>
       <c r="J13" s="20">
-        <f t="shared" ref="J13" si="8">I13*D13*25</f>
-        <v>574.5</v>
+        <f t="shared" ref="J13" si="10">I13*D13*25</f>
+        <v>572.32500000000005</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>17</v>
@@ -2127,21 +2319,32 @@
       </c>
       <c r="P13" s="58">
         <f t="shared" si="3"/>
-        <v>0.30557959782179134</v>
+        <v>0.29721854497846539</v>
       </c>
       <c r="Q13" s="59">
         <f t="shared" si="4"/>
-        <v>0.3047765154550785</v>
+        <v>0.29633365829911151</v>
       </c>
       <c r="R13" s="60">
         <f t="shared" si="5"/>
-        <v>0.29604741911837645</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>0.28991068273946791</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T13" s="82">
+        <f>'Shield Parts'!U$32</f>
+        <v>0</v>
+      </c>
+      <c r="U13" s="84">
+        <f>'Shield Parts'!U31</f>
+        <v>474.392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>17</v>
@@ -2174,34 +2377,45 @@
         <v>18</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M14" s="29" t="s">
         <v>17</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="O14" s="44" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="P14" s="58">
         <f t="shared" si="3"/>
-        <v>2.4008066710414708E-3</v>
+        <v>2.3704546532024853E-3</v>
       </c>
       <c r="Q14" s="59">
         <f t="shared" si="4"/>
-        <v>2.480546788836776E-3</v>
+        <v>2.4466535425661257E-3</v>
       </c>
       <c r="R14" s="60">
         <f t="shared" si="5"/>
-        <v>2.3833234350260947E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+        <v>2.3427893376491318E-3</v>
+      </c>
+      <c r="S14" s="2">
+        <v>6</v>
+      </c>
+      <c r="T14" s="82">
+        <f>E14</f>
+        <v>1.95</v>
+      </c>
+      <c r="U14" s="84">
+        <f t="shared" si="7"/>
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="25" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>17</v>
@@ -2231,7 +2445,7 @@
         <v>150</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L15" s="25" t="s">
         <v>17</v>
@@ -2241,25 +2455,36 @@
       </c>
       <c r="N15" s="19"/>
       <c r="O15" s="44" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="P15" s="58">
         <f t="shared" si="3"/>
-        <v>7.3870974493583708E-2</v>
+        <v>7.2937066252384164E-2</v>
       </c>
       <c r="Q15" s="59">
         <f t="shared" si="4"/>
-        <v>7.6324516579593105E-2</v>
+        <v>7.528164746357309E-2</v>
       </c>
       <c r="R15" s="60">
         <f t="shared" si="5"/>
-        <v>7.7296976271116577E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+        <v>7.5982356896728581E-2</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0</v>
+      </c>
+      <c r="T15" s="82">
+        <f>E15</f>
+        <v>6</v>
+      </c>
+      <c r="U15" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="25" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>17</v>
@@ -2289,37 +2514,47 @@
         <v>1.9449999999999998</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="M16" s="32" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="N16" s="27" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="O16" s="44" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="P16" s="58">
         <f t="shared" si="3"/>
-        <v>9.5786030260013543E-4</v>
+        <v>9.4575062573924783E-4</v>
       </c>
       <c r="Q16" s="59">
         <f t="shared" si="4"/>
-        <v>9.8967456498205708E-4</v>
+        <v>9.7615202877766427E-4</v>
       </c>
       <c r="R16" s="60">
         <f t="shared" si="5"/>
-        <v>1.0022841256488114E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+        <v>9.8523789442758053E-4</v>
+      </c>
+      <c r="S16" s="2">
+        <v>1</v>
+      </c>
+      <c r="T16" s="82">
+        <v>7.78</v>
+      </c>
+      <c r="U16" s="84">
+        <f t="shared" si="7"/>
+        <v>7.78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="25" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>17</v>
@@ -2350,34 +2585,44 @@
         <v>0.74750000000000005</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="L17" s="29">
         <v>203286992</v>
       </c>
       <c r="M17" s="29" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="N17" s="19" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="O17" s="44" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="P17" s="58">
         <f t="shared" si="3"/>
-        <v>3.6812368955969221E-4</v>
+        <v>3.6346971349104776E-4</v>
       </c>
       <c r="Q17" s="59">
         <f t="shared" si="4"/>
-        <v>3.8035050762163906E-4</v>
+        <v>3.751535431934726E-4</v>
       </c>
       <c r="R17" s="60">
         <f t="shared" si="5"/>
-        <v>3.8519659841773093E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+        <v>3.7864541186869745E-4</v>
+      </c>
+      <c r="S17" s="2">
+        <v>2</v>
+      </c>
+      <c r="T17" s="82">
+        <v>5.98</v>
+      </c>
+      <c r="U17" s="84">
+        <f t="shared" si="7"/>
+        <v>11.96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
@@ -2414,8 +2659,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S18" s="2">
+        <f>$T$1*D18</f>
+        <v>0</v>
+      </c>
+      <c r="T18" s="82"/>
+      <c r="U18" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="34"/>
       <c r="C19" s="25"/>
@@ -2452,8 +2706,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S19" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T19" s="82"/>
+      <c r="U19" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
@@ -2490,8 +2753,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S20" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T20" s="82"/>
+      <c r="U20" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
@@ -2528,8 +2800,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S21" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T21" s="82"/>
+      <c r="U21" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
@@ -2566,8 +2847,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S22" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T22" s="82"/>
+      <c r="U22" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
@@ -2604,8 +2894,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S23" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T23" s="82"/>
+      <c r="U23" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
@@ -2642,8 +2941,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S24" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T24" s="82"/>
+      <c r="U24" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="25"/>
       <c r="C25" s="25"/>
@@ -2680,8 +2988,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S25" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T25" s="82"/>
+      <c r="U25" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2718,8 +3035,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S26" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T26" s="82"/>
+      <c r="U26" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2756,8 +3082,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S27" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T27" s="82"/>
+      <c r="U27" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2794,8 +3129,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S28" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T28" s="82"/>
+      <c r="U28" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2832,8 +3176,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S29" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T29" s="82"/>
+      <c r="U29" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="46"/>
       <c r="B30" s="47"/>
       <c r="C30" s="47"/>
@@ -2870,69 +3223,87 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S30" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T30" s="83"/>
+      <c r="U30" s="85">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="E31" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
-        <v>81.222699999999975</v>
+        <v>82.262699999999967</v>
       </c>
       <c r="G31" s="24" t="s">
         <v>14</v>
       </c>
       <c r="H31" s="24">
         <f>SUM(H4:H30)</f>
-        <v>786.11700000000008</v>
+        <v>797.00700000000006</v>
       </c>
       <c r="I31" s="24" t="s">
         <v>14</v>
       </c>
       <c r="J31" s="24">
         <f>SUM(J4:J30)</f>
-        <v>1940.5674999999999</v>
+        <v>1974.1424999999999</v>
       </c>
       <c r="M31" s="30"/>
       <c r="P31" s="64">
         <f>SUM(P4:P30)</f>
-        <v>1.0000000000000004</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="Q31" s="64">
-        <f t="shared" ref="Q31:R31" si="9">SUM(Q4:Q30)</f>
-        <v>0.99999999999999978</v>
+        <f t="shared" ref="Q31:R31" si="11">SUM(Q4:Q30)</f>
+        <v>1</v>
       </c>
       <c r="R31" s="64">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T31" t="s">
+        <v>157</v>
+      </c>
+      <c r="U31" s="86">
+        <f>SUM(U4:U30)</f>
+        <v>3266.8959999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
         <v>15</v>
       </c>
       <c r="F32" s="24">
         <f>F31</f>
-        <v>81.222699999999975</v>
+        <v>82.262699999999967</v>
       </c>
       <c r="G32" t="s">
         <v>15</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
-        <v>78.611700000000013</v>
+        <v>79.700700000000012</v>
       </c>
       <c r="I32" t="s">
         <v>15</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
-        <v>77.622699999999995</v>
+        <v>78.965699999999998</v>
       </c>
       <c r="M32" s="30"/>
+      <c r="U32" s="86"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="S2:U2"/>
     <mergeCell ref="P2:R2"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="A1:B1"/>
@@ -2948,10 +3319,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2971,9 +3342,11 @@
     <col min="13" max="13" width="28" style="30" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="130.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="94" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
         <v>10</v>
       </c>
@@ -2984,8 +3357,15 @@
       <c r="D1" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>154</v>
+      </c>
+      <c r="T1">
+        <f>'Full Instrument'!T1</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
         <v>6</v>
       </c>
@@ -3013,13 +3393,23 @@
       <c r="O2" s="77" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="T2" s="66"/>
+      <c r="U2" s="67"/>
+    </row>
+    <row r="3" spans="1:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>1</v>
@@ -3058,8 +3448,26 @@
         <v>4</v>
       </c>
       <c r="O3" s="78"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q3" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="R3" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="S3" s="80" t="s">
+        <v>151</v>
+      </c>
+      <c r="T3" s="81" t="s">
+        <v>152</v>
+      </c>
+      <c r="U3" s="79" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>17</v>
@@ -3106,11 +3514,34 @@
       <c r="O4" s="43" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4" s="58">
+        <f>F4/$F$31</f>
+        <v>0.40695296523517388</v>
+      </c>
+      <c r="Q4" s="59">
+        <f>H4/$H$31</f>
+        <v>0.40011855364552462</v>
+      </c>
+      <c r="R4" s="60">
+        <f>J4/$J$31</f>
+        <v>0.39138601319180538</v>
+      </c>
+      <c r="S4" s="8">
+        <v>12</v>
+      </c>
+      <c r="T4" s="87">
+        <f>G4</f>
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="U4" s="88">
+        <f>S4*T4</f>
+        <v>113.39999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="25" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>19</v>
@@ -3152,11 +3583,35 @@
         <v>21</v>
       </c>
       <c r="O5" s="44"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5" s="58">
+        <f t="shared" ref="P5:P30" si="3">F5/$F$31</f>
+        <v>6.1349693251533756E-2</v>
+      </c>
+      <c r="Q5" s="59">
+        <f t="shared" ref="Q5:Q30" si="4">H5/$H$31</f>
+        <v>6.3510881531035651E-2</v>
+      </c>
+      <c r="R5" s="60">
+        <f t="shared" ref="R5:R30" si="5">J5/$J$31</f>
+        <v>6.2464508801817142E-2</v>
+      </c>
+      <c r="S5" s="2">
+        <f t="shared" ref="S5:S30" si="6">$T$1*D5</f>
+        <v>58</v>
+      </c>
+      <c r="T5" s="82">
+        <f>I5</f>
+        <v>1.43</v>
+      </c>
+      <c r="U5" s="84">
+        <f t="shared" ref="U5:U30" si="7">S5*T5</f>
+        <v>82.94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>22</v>
@@ -3165,25 +3620,25 @@
         <v>1</v>
       </c>
       <c r="E6" s="38">
-        <v>1.74</v>
+        <v>1.39</v>
       </c>
       <c r="F6" s="26">
         <f>D6*E6</f>
-        <v>1.74</v>
+        <v>1.39</v>
       </c>
       <c r="G6" s="21">
-        <v>1.74</v>
+        <v>1.39</v>
       </c>
       <c r="H6" s="20">
-        <f t="shared" ref="H6:H30" si="3">D6*G6*10</f>
-        <v>17.399999999999999</v>
+        <f t="shared" ref="H6:H30" si="8">D6*G6*10</f>
+        <v>13.899999999999999</v>
       </c>
       <c r="I6" s="21">
-        <v>1.49</v>
+        <v>1.39</v>
       </c>
       <c r="J6" s="20">
         <f>D6*I6*25</f>
-        <v>37.25</v>
+        <v>34.75</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>23</v>
@@ -3198,13 +3653,37 @@
         <v>25</v>
       </c>
       <c r="O6" s="44" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="P6" s="58">
+        <f t="shared" si="3"/>
+        <v>5.6850715746421275E-2</v>
+      </c>
+      <c r="Q6" s="59">
+        <f t="shared" si="4"/>
+        <v>5.885341688542637E-2</v>
+      </c>
+      <c r="R6" s="60">
+        <f t="shared" si="5"/>
+        <v>6.0717249814353731E-2</v>
+      </c>
+      <c r="S6" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T6" s="82">
+        <f>E6</f>
+        <v>1.39</v>
+      </c>
+      <c r="U6" s="84">
+        <f t="shared" si="7"/>
+        <v>80.61999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>38</v>
@@ -3216,21 +3695,21 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="26">
-        <f t="shared" ref="F7:F30" si="4">D7*E7</f>
+        <f t="shared" ref="F7:F30" si="9">D7*E7</f>
         <v>0.5</v>
       </c>
       <c r="G7" s="21">
         <v>0.5</v>
       </c>
       <c r="H7" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="I7" s="21">
         <v>0.48</v>
       </c>
       <c r="J7" s="20">
-        <f t="shared" ref="J7:J30" si="5">D7*I7*25</f>
+        <f t="shared" ref="J7:J30" si="10">D7*I7*25</f>
         <v>12</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -3246,11 +3725,35 @@
         <v>41</v>
       </c>
       <c r="O7" s="44"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P7" s="58">
+        <f t="shared" si="3"/>
+        <v>2.0449897750511252E-2</v>
+      </c>
+      <c r="Q7" s="59">
+        <f t="shared" si="4"/>
+        <v>2.1170293843678554E-2</v>
+      </c>
+      <c r="R7" s="60">
+        <f t="shared" si="5"/>
+        <v>2.0967107849561E-2</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T7" s="82">
+        <f>I7</f>
+        <v>0.48</v>
+      </c>
+      <c r="U7" s="84">
+        <f t="shared" si="7"/>
+        <v>27.84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>42</v>
@@ -3262,21 +3765,21 @@
         <v>0.43</v>
       </c>
       <c r="F8" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.43</v>
       </c>
       <c r="G8" s="21">
         <v>0.43</v>
       </c>
       <c r="H8" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>4.3</v>
       </c>
       <c r="I8" s="21">
         <v>0.35699999999999998</v>
       </c>
       <c r="J8" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.9249999999999989</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -3294,8 +3797,31 @@
       <c r="O8" s="44" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P8" s="58">
+        <f t="shared" si="3"/>
+        <v>1.7586912065439674E-2</v>
+      </c>
+      <c r="Q8" s="59">
+        <f t="shared" si="4"/>
+        <v>1.8206452705563553E-2</v>
+      </c>
+      <c r="R8" s="60">
+        <f t="shared" si="5"/>
+        <v>1.5594286463110991E-2</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T8" s="82">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="U8" s="84">
+        <f t="shared" si="7"/>
+        <v>18.966000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="25" t="s">
         <v>17</v>
@@ -3310,21 +3836,21 @@
         <v>1.5</v>
       </c>
       <c r="F9" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.5</v>
       </c>
       <c r="G9" s="21">
         <v>1.5</v>
       </c>
       <c r="H9" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="I9" s="21">
         <v>1.43</v>
       </c>
       <c r="J9" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>35.75</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -3334,7 +3860,7 @@
         <v>52</v>
       </c>
       <c r="M9" s="32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N9" s="19" t="s">
         <v>53</v>
@@ -3342,11 +3868,35 @@
       <c r="O9" s="44" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P9" s="58">
+        <f t="shared" si="3"/>
+        <v>6.1349693251533756E-2</v>
+      </c>
+      <c r="Q9" s="59">
+        <f t="shared" si="4"/>
+        <v>6.3510881531035651E-2</v>
+      </c>
+      <c r="R9" s="60">
+        <f t="shared" si="5"/>
+        <v>6.2464508801817142E-2</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T9" s="82">
+        <f>I9</f>
+        <v>1.43</v>
+      </c>
+      <c r="U9" s="84">
+        <f t="shared" si="7"/>
+        <v>82.94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>55</v>
@@ -3358,21 +3908,21 @@
         <v>0.13</v>
       </c>
       <c r="F10" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.13</v>
       </c>
       <c r="G10" s="21">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="H10" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.79</v>
       </c>
       <c r="I10" s="21">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="J10" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>1.9750000000000001</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -3390,11 +3940,34 @@
       <c r="O10" s="44" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10" s="58">
+        <f t="shared" si="3"/>
+        <v>5.3169734151329254E-3</v>
+      </c>
+      <c r="Q10" s="59">
+        <f t="shared" si="4"/>
+        <v>3.3449064273012113E-3</v>
+      </c>
+      <c r="R10" s="60">
+        <f t="shared" si="5"/>
+        <v>3.4508365002402482E-3</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T10" s="82">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="U10" s="84">
+        <f>S10*T10</f>
+        <v>4.5819999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>60</v>
@@ -3406,21 +3979,21 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F11" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="G11" s="21">
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="H11" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.85999999999999988</v>
       </c>
       <c r="I11" s="21">
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="J11" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.15</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -3438,11 +4011,34 @@
       <c r="O11" s="44" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P11" s="58">
+        <f t="shared" si="3"/>
+        <v>5.7259713701431512E-3</v>
+      </c>
+      <c r="Q11" s="59">
+        <f t="shared" si="4"/>
+        <v>3.6412905411127103E-3</v>
+      </c>
+      <c r="R11" s="60">
+        <f t="shared" si="5"/>
+        <v>3.7566068230463455E-3</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T11" s="82">
+        <v>0.86</v>
+      </c>
+      <c r="U11" s="84">
+        <f t="shared" ref="U11:U15" si="11">S11*T11</f>
+        <v>49.88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="34" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>63</v>
@@ -3451,46 +4047,69 @@
         <v>1</v>
       </c>
       <c r="E12" s="38">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="F12" s="26">
-        <f t="shared" si="4"/>
-        <v>0.12</v>
+        <f t="shared" si="9"/>
+        <v>0.1</v>
       </c>
       <c r="G12" s="21">
-        <v>0.02</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="H12" s="20">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
+        <f t="shared" si="8"/>
+        <v>0.29000000000000004</v>
       </c>
       <c r="I12" s="21">
-        <v>1.6E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="J12" s="20">
-        <f t="shared" si="5"/>
-        <v>0.4</v>
+        <f t="shared" si="10"/>
+        <v>0.72500000000000009</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>56</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>101</v>
+        <v>159</v>
       </c>
       <c r="M12" s="29" t="s">
         <v>17</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>102</v>
+        <v>160</v>
       </c>
       <c r="O12" s="44" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P12" s="58">
+        <f t="shared" si="3"/>
+        <v>4.0899795501022507E-3</v>
+      </c>
+      <c r="Q12" s="59">
+        <f t="shared" si="4"/>
+        <v>1.2278770429333561E-3</v>
+      </c>
+      <c r="R12" s="60">
+        <f t="shared" si="5"/>
+        <v>1.2667627659109773E-3</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T12" s="82">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="U12" s="84">
+        <f t="shared" si="11"/>
+        <v>1.6820000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>66</v>
@@ -3502,43 +4121,66 @@
         <v>0.12</v>
       </c>
       <c r="F13" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.12</v>
       </c>
       <c r="G13" s="21">
         <v>0.02</v>
       </c>
       <c r="H13" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.2</v>
       </c>
       <c r="I13" s="21">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="J13" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>56</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M13" s="29" t="s">
         <v>17</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O13" s="44" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P13" s="58">
+        <f t="shared" si="3"/>
+        <v>4.9079754601226997E-3</v>
+      </c>
+      <c r="Q13" s="59">
+        <f t="shared" si="4"/>
+        <v>8.4681175374714212E-4</v>
+      </c>
+      <c r="R13" s="60">
+        <f t="shared" si="5"/>
+        <v>7.862665443585374E-4</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T13" s="82">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="U13" s="84">
+        <f t="shared" si="11"/>
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>80</v>
@@ -3550,43 +4192,66 @@
         <v>0.12</v>
       </c>
       <c r="F14" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.12</v>
       </c>
       <c r="G14" s="21">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="H14" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.91999999999999993</v>
       </c>
       <c r="I14" s="21">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="J14" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>56</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M14" s="29" t="s">
         <v>17</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="O14" s="44" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P14" s="58">
+        <f t="shared" si="3"/>
+        <v>4.9079754601226997E-3</v>
+      </c>
+      <c r="Q14" s="59">
+        <f t="shared" si="4"/>
+        <v>3.8953340672368531E-3</v>
+      </c>
+      <c r="R14" s="60">
+        <f t="shared" si="5"/>
+        <v>4.0186956711658582E-3</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T14" s="82">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="U14" s="84">
+        <f t="shared" si="11"/>
+        <v>5.3360000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="25" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>81</v>
@@ -3598,40 +4263,63 @@
         <v>0.12</v>
       </c>
       <c r="F15" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.12</v>
       </c>
       <c r="G15" s="21">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="H15" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.91999999999999993</v>
       </c>
       <c r="I15" s="21">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="J15" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>56</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M15" s="29" t="s">
         <v>17</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O15" s="44" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P15" s="58">
+        <f t="shared" si="3"/>
+        <v>4.9079754601226997E-3</v>
+      </c>
+      <c r="Q15" s="59">
+        <f t="shared" si="4"/>
+        <v>3.8953340672368531E-3</v>
+      </c>
+      <c r="R15" s="60">
+        <f t="shared" si="5"/>
+        <v>4.0186956711658582E-3</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T15" s="82">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="U15" s="84">
+        <f t="shared" si="11"/>
+        <v>5.3360000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="25" t="s">
         <v>17</v>
@@ -3646,21 +4334,21 @@
         <v>8.4499999999999993</v>
       </c>
       <c r="F16" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>8.4499999999999993</v>
       </c>
       <c r="G16" s="21">
         <v>8.4499999999999993</v>
       </c>
       <c r="H16" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>84.5</v>
       </c>
       <c r="I16" s="21">
         <v>8.4499999999999993</v>
       </c>
       <c r="J16" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>211.24999999999997</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -3676,25 +4364,46 @@
       <c r="O16" s="44" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P16" s="58">
+        <f t="shared" si="3"/>
+        <v>0.3456032719836401</v>
+      </c>
+      <c r="Q16" s="59">
+        <f t="shared" si="4"/>
+        <v>0.35777796595816752</v>
+      </c>
+      <c r="R16" s="60">
+        <f t="shared" si="5"/>
+        <v>0.36910846110164669</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="T16" s="82"/>
+      <c r="U16" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
       <c r="D17" s="4"/>
       <c r="E17" s="38"/>
       <c r="F17" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I17" s="21"/>
       <c r="J17" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K17" s="2"/>
@@ -3702,25 +4411,46 @@
       <c r="M17" s="29"/>
       <c r="N17" s="19"/>
       <c r="O17" s="44"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P17" s="58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R17" s="60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T17" s="82"/>
+      <c r="U17" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="4"/>
       <c r="E18" s="38"/>
       <c r="F18" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I18" s="21"/>
       <c r="J18" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K18" s="2"/>
@@ -3728,25 +4458,46 @@
       <c r="M18" s="29"/>
       <c r="N18" s="19"/>
       <c r="O18" s="44"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P18" s="58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T18" s="82"/>
+      <c r="U18" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="34"/>
       <c r="C19" s="25"/>
       <c r="D19" s="4"/>
       <c r="E19" s="38"/>
       <c r="F19" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G19" s="21"/>
       <c r="H19" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I19" s="21"/>
       <c r="J19" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K19" s="2"/>
@@ -3754,25 +4505,46 @@
       <c r="M19" s="29"/>
       <c r="N19" s="19"/>
       <c r="O19" s="44"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P19" s="58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T19" s="82"/>
+      <c r="U19" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
       <c r="D20" s="4"/>
       <c r="E20" s="38"/>
       <c r="F20" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G20" s="21"/>
       <c r="H20" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I20" s="21"/>
       <c r="J20" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K20" s="2"/>
@@ -3780,25 +4552,46 @@
       <c r="M20" s="29"/>
       <c r="N20" s="19"/>
       <c r="O20" s="44"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P20" s="58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T20" s="82"/>
+      <c r="U20" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
       <c r="D21" s="4"/>
       <c r="E21" s="38"/>
       <c r="F21" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G21" s="21"/>
       <c r="H21" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I21" s="21"/>
       <c r="J21" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K21" s="2"/>
@@ -3806,25 +4599,46 @@
       <c r="M21" s="29"/>
       <c r="N21" s="19"/>
       <c r="O21" s="44"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P21" s="58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S21" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T21" s="82"/>
+      <c r="U21" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
       <c r="D22" s="4"/>
       <c r="E22" s="38"/>
       <c r="F22" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G22" s="21"/>
       <c r="H22" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I22" s="21"/>
       <c r="J22" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K22" s="2"/>
@@ -3832,25 +4646,46 @@
       <c r="M22" s="29"/>
       <c r="N22" s="19"/>
       <c r="O22" s="44"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P22" s="58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S22" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T22" s="82"/>
+      <c r="U22" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
       <c r="D23" s="4"/>
       <c r="E23" s="38"/>
       <c r="F23" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G23" s="21"/>
       <c r="H23" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I23" s="21"/>
       <c r="J23" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K23" s="2"/>
@@ -3858,25 +4693,46 @@
       <c r="M23" s="29"/>
       <c r="N23" s="19"/>
       <c r="O23" s="44"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P23" s="58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S23" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T23" s="82"/>
+      <c r="U23" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
       <c r="D24" s="4"/>
       <c r="E24" s="38"/>
       <c r="F24" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G24" s="21"/>
       <c r="H24" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I24" s="21"/>
       <c r="J24" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K24" s="2"/>
@@ -3884,25 +4740,46 @@
       <c r="M24" s="29"/>
       <c r="N24" s="19"/>
       <c r="O24" s="44"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P24" s="58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S24" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T24" s="82"/>
+      <c r="U24" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="25"/>
       <c r="C25" s="25"/>
       <c r="D25" s="4"/>
       <c r="E25" s="38"/>
       <c r="F25" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G25" s="21"/>
       <c r="H25" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I25" s="21"/>
       <c r="J25" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K25" s="2"/>
@@ -3910,25 +4787,46 @@
       <c r="M25" s="29"/>
       <c r="N25" s="19"/>
       <c r="O25" s="44"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P25" s="58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S25" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T25" s="82"/>
+      <c r="U25" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
       <c r="E26" s="38"/>
       <c r="F26" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G26" s="21"/>
       <c r="H26" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I26" s="21"/>
       <c r="J26" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K26" s="2"/>
@@ -3936,25 +4834,46 @@
       <c r="M26" s="29"/>
       <c r="N26" s="4"/>
       <c r="O26" s="44"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P26" s="58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R26" s="60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S26" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T26" s="82"/>
+      <c r="U26" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="4"/>
       <c r="E27" s="38"/>
       <c r="F27" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G27" s="21"/>
       <c r="H27" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I27" s="21"/>
       <c r="J27" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K27" s="2"/>
@@ -3962,25 +4881,46 @@
       <c r="M27" s="29"/>
       <c r="N27" s="4"/>
       <c r="O27" s="44"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P27" s="58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S27" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T27" s="82"/>
+      <c r="U27" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
       <c r="E28" s="38"/>
       <c r="F28" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G28" s="21"/>
       <c r="H28" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I28" s="21"/>
       <c r="J28" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K28" s="2"/>
@@ -3988,25 +4928,46 @@
       <c r="M28" s="29"/>
       <c r="N28" s="4"/>
       <c r="O28" s="44"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P28" s="58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R28" s="60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S28" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T28" s="82"/>
+      <c r="U28" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="4"/>
       <c r="E29" s="38"/>
       <c r="F29" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G29" s="21"/>
       <c r="H29" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I29" s="21"/>
       <c r="J29" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K29" s="2"/>
@@ -4014,25 +4975,46 @@
       <c r="M29" s="29"/>
       <c r="N29" s="4"/>
       <c r="O29" s="44"/>
-    </row>
-    <row r="30" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P29" s="58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S29" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T29" s="82"/>
+      <c r="U29" s="84">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
       <c r="E30" s="39"/>
       <c r="F30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G30" s="23"/>
       <c r="H30" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I30" s="23"/>
       <c r="J30" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K30" s="5"/>
@@ -4040,55 +5022,98 @@
       <c r="M30" s="33"/>
       <c r="N30" s="7"/>
       <c r="O30" s="45"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P30" s="61">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="62">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R30" s="63">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S30" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T30" s="83"/>
+      <c r="U30" s="85">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="E31" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
-        <v>24.820000000000004</v>
+        <v>24.449999999999996</v>
       </c>
       <c r="G31" s="24" t="s">
         <v>14</v>
       </c>
       <c r="H31" s="24">
         <f>SUM(H4:H30)</f>
-        <v>239.58999999999997</v>
+        <v>236.17999999999998</v>
       </c>
       <c r="I31" s="24" t="s">
         <v>14</v>
       </c>
       <c r="J31" s="24">
         <f>SUM(J4:J30)</f>
-        <v>574.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+        <v>572.32500000000005</v>
+      </c>
+      <c r="P31" s="64">
+        <f>SUM(P4:P30)</f>
+        <v>1</v>
+      </c>
+      <c r="Q31" s="64">
+        <f t="shared" ref="Q31:R31" si="12">SUM(Q4:Q30)</f>
+        <v>1</v>
+      </c>
+      <c r="R31" s="64">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="T31" t="s">
+        <v>157</v>
+      </c>
+      <c r="U31" s="86">
+        <f>SUM(U4:U30)</f>
+        <v>474.392</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
         <v>15</v>
       </c>
       <c r="F32" s="24">
         <f>F31</f>
-        <v>24.820000000000004</v>
+        <v>24.449999999999996</v>
       </c>
       <c r="G32" t="s">
         <v>15</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
-        <v>23.958999999999996</v>
+        <v>23.617999999999999</v>
       </c>
       <c r="I32" t="s">
         <v>15</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
-        <v>22.98</v>
-      </c>
+        <v>22.893000000000001</v>
+      </c>
+      <c r="U32" s="86"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:U2"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Added PCB costs to BOM
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Full Instrument" sheetId="3" r:id="rId1"/>
@@ -283,9 +283,6 @@
     <t>OshPark</t>
   </si>
   <si>
-    <t>Currently using OshPark Prices @ $8.45 for 2"x2.5" board ($5/in^2). Will change once quantity price is determined</t>
-  </si>
-  <si>
     <t>Jumper Wires</t>
   </si>
   <si>
@@ -512,6 +509,9 @@
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/TE-Connectivity-Neohm/CFR25J270R/?qs=sGAEpiMZZMu61qfTUdNhG05q5R9Z8%252b9s90AksAri%2fIw%3d</t>
+  </si>
+  <si>
+    <t>2"x2.5" board. $5/in^2 for regular order, $1/in^2 for medium run.</t>
   </si>
 </sst>
 </file>
@@ -1076,6 +1076,16 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="20" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="20" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="26" xfId="20" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1118,16 +1128,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="20" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="20" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="26" xfId="20" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Currency" xfId="20" builtinId="4"/>
@@ -1486,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1512,10 +1512,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="71"/>
+      <c r="B1" s="81"/>
       <c r="C1" s="1">
         <v>1</v>
       </c>
@@ -1524,50 +1524,50 @@
       </c>
       <c r="M1" s="30"/>
       <c r="S1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T1">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="74"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="84"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="72" t="s">
+      <c r="E2" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="75"/>
-      <c r="G2" s="76" t="s">
+      <c r="F2" s="85"/>
+      <c r="G2" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="75"/>
-      <c r="I2" s="72" t="s">
+      <c r="H2" s="85"/>
+      <c r="I2" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="75"/>
-      <c r="K2" s="72" t="s">
+      <c r="J2" s="85"/>
+      <c r="K2" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="73"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="68" t="s">
+      <c r="L2" s="83"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="65" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="65" t="s">
-        <v>150</v>
-      </c>
-      <c r="T2" s="66"/>
-      <c r="U2" s="67"/>
+      <c r="P2" s="75" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="T2" s="76"/>
+      <c r="U2" s="77"/>
     </row>
     <row r="3" spans="1:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -1580,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>68</v>
@@ -1612,24 +1612,24 @@
       <c r="N3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="69"/>
+      <c r="O3" s="79"/>
       <c r="P3" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q3" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="Q3" s="56" t="s">
+      <c r="R3" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="R3" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="S3" s="80" t="s">
+      <c r="S3" s="66" t="s">
+        <v>150</v>
+      </c>
+      <c r="T3" s="67" t="s">
         <v>151</v>
       </c>
-      <c r="T3" s="81" t="s">
+      <c r="U3" s="65" t="s">
         <v>152</v>
-      </c>
-      <c r="U3" s="79" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -1638,7 +1638,7 @@
         <v>33</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -1668,7 +1668,7 @@
         <v>27</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M4" s="29" t="s">
         <v>28</v>
@@ -1693,11 +1693,11 @@
         <f>$T$1*D4</f>
         <v>58</v>
       </c>
-      <c r="T4" s="82">
+      <c r="T4" s="68">
         <f>E4</f>
         <v>6.5</v>
       </c>
-      <c r="U4" s="84">
+      <c r="U4" s="70">
         <f>S4*T4</f>
         <v>377</v>
       </c>
@@ -1765,11 +1765,11 @@
         <f t="shared" ref="S5:S30" si="6">$T$1*D5</f>
         <v>58</v>
       </c>
-      <c r="T5" s="82">
+      <c r="T5" s="68">
         <f>E5</f>
         <v>11.2</v>
       </c>
-      <c r="U5" s="84">
+      <c r="U5" s="70">
         <f t="shared" ref="U5:U30" si="7">S5*T5</f>
         <v>649.59999999999991</v>
       </c>
@@ -1835,11 +1835,11 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T6" s="82">
+      <c r="T6" s="68">
         <f>E6</f>
         <v>10.5</v>
       </c>
-      <c r="U6" s="84">
+      <c r="U6" s="70">
         <f t="shared" si="7"/>
         <v>609</v>
       </c>
@@ -1905,11 +1905,11 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T7" s="82">
+      <c r="T7" s="68">
         <f>G7</f>
         <v>12.56</v>
       </c>
-      <c r="U7" s="84">
+      <c r="U7" s="70">
         <f t="shared" si="7"/>
         <v>728.48</v>
       </c>
@@ -1950,16 +1950,16 @@
         <v>56</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="M8" s="32" t="s">
+      <c r="N8" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="N8" s="19" t="s">
+      <c r="O8" s="44" t="s">
         <v>99</v>
-      </c>
-      <c r="O8" s="44" t="s">
-        <v>100</v>
       </c>
       <c r="P8" s="58">
         <f t="shared" si="3"/>
@@ -1977,10 +1977,10 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T8" s="82">
+      <c r="T8" s="68">
         <v>0.7</v>
       </c>
-      <c r="U8" s="84">
+      <c r="U8" s="70">
         <f t="shared" si="7"/>
         <v>40.599999999999994</v>
       </c>
@@ -2021,16 +2021,16 @@
         <v>56</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M9" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="N9" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="N9" s="19" t="s">
+      <c r="O9" s="44" t="s">
         <v>88</v>
-      </c>
-      <c r="O9" s="44" t="s">
-        <v>89</v>
       </c>
       <c r="P9" s="58">
         <f t="shared" si="3"/>
@@ -2047,10 +2047,10 @@
       <c r="S9" s="2">
         <v>0</v>
       </c>
-      <c r="T9" s="82">
+      <c r="T9" s="68">
         <v>0.23</v>
       </c>
-      <c r="U9" s="84">
+      <c r="U9" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2058,7 +2058,7 @@
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>17</v>
@@ -2097,10 +2097,10 @@
         <v>17</v>
       </c>
       <c r="N10" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="O10" s="44" t="s">
         <v>118</v>
-      </c>
-      <c r="O10" s="44" t="s">
-        <v>119</v>
       </c>
       <c r="P10" s="58">
         <f t="shared" si="3"/>
@@ -2117,11 +2117,11 @@
       <c r="S10" s="2">
         <v>12</v>
       </c>
-      <c r="T10" s="82">
+      <c r="T10" s="68">
         <f>G10</f>
         <v>3.56</v>
       </c>
-      <c r="U10" s="84">
+      <c r="U10" s="70">
         <f t="shared" si="7"/>
         <v>42.72</v>
       </c>
@@ -2129,7 +2129,7 @@
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>17</v>
@@ -2162,16 +2162,16 @@
         <v>56</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M11" s="32" t="s">
         <v>17</v>
       </c>
       <c r="N11" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="O11" s="44" t="s">
         <v>91</v>
-      </c>
-      <c r="O11" s="44" t="s">
-        <v>92</v>
       </c>
       <c r="P11" s="58">
         <f t="shared" si="3"/>
@@ -2189,10 +2189,10 @@
         <f t="shared" si="6"/>
         <v>116</v>
       </c>
-      <c r="T11" s="82">
+      <c r="T11" s="68">
         <v>0.90400000000000003</v>
       </c>
-      <c r="U11" s="84">
+      <c r="U11" s="70">
         <f t="shared" si="7"/>
         <v>104.864</v>
       </c>
@@ -2200,7 +2200,7 @@
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>17</v>
@@ -2230,19 +2230,19 @@
         <v>90</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="M12" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="N12" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="M12" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="N12" s="19" t="s">
-        <v>156</v>
-      </c>
       <c r="O12" s="44" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P12" s="58">
         <f t="shared" si="3"/>
@@ -2260,11 +2260,11 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T12" s="82">
+      <c r="T12" s="68">
         <f>E12</f>
         <v>3.6</v>
       </c>
-      <c r="U12" s="84">
+      <c r="U12" s="70">
         <f t="shared" si="7"/>
         <v>208.8</v>
       </c>
@@ -2272,7 +2272,7 @@
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>17</v>
@@ -2305,7 +2305,7 @@
         <v>572.32500000000005</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>17</v>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="N13" s="19"/>
       <c r="O13" s="44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P13" s="58">
         <f t="shared" si="3"/>
@@ -2332,19 +2332,19 @@
       <c r="S13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T13" s="82">
+      <c r="T13" s="68">
         <f>'Shield Parts'!U$32</f>
         <v>0</v>
       </c>
-      <c r="U13" s="84">
+      <c r="U13" s="70">
         <f>'Shield Parts'!U31</f>
-        <v>474.392</v>
+        <v>778.5920000000001</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>17</v>
@@ -2377,16 +2377,16 @@
         <v>18</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M14" s="29" t="s">
         <v>17</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O14" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P14" s="58">
         <f t="shared" si="3"/>
@@ -2403,11 +2403,11 @@
       <c r="S14" s="2">
         <v>6</v>
       </c>
-      <c r="T14" s="82">
+      <c r="T14" s="68">
         <f>E14</f>
         <v>1.95</v>
       </c>
-      <c r="U14" s="84">
+      <c r="U14" s="70">
         <f t="shared" si="7"/>
         <v>11.7</v>
       </c>
@@ -2415,7 +2415,7 @@
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>17</v>
@@ -2445,7 +2445,7 @@
         <v>150</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L15" s="25" t="s">
         <v>17</v>
@@ -2455,7 +2455,7 @@
       </c>
       <c r="N15" s="19"/>
       <c r="O15" s="44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P15" s="58">
         <f t="shared" si="3"/>
@@ -2472,11 +2472,11 @@
       <c r="S15" s="2">
         <v>0</v>
       </c>
-      <c r="T15" s="82">
+      <c r="T15" s="68">
         <f>E15</f>
         <v>6</v>
       </c>
-      <c r="U15" s="84">
+      <c r="U15" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2484,7 +2484,7 @@
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>17</v>
@@ -2514,19 +2514,19 @@
         <v>1.9449999999999998</v>
       </c>
       <c r="K16" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="M16" s="32" t="s">
+      <c r="N16" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="N16" s="27" t="s">
+      <c r="O16" s="44" t="s">
         <v>131</v>
-      </c>
-      <c r="O16" s="44" t="s">
-        <v>132</v>
       </c>
       <c r="P16" s="58">
         <f t="shared" si="3"/>
@@ -2543,10 +2543,10 @@
       <c r="S16" s="2">
         <v>1</v>
       </c>
-      <c r="T16" s="82">
+      <c r="T16" s="68">
         <v>7.78</v>
       </c>
-      <c r="U16" s="84">
+      <c r="U16" s="70">
         <f t="shared" si="7"/>
         <v>7.78</v>
       </c>
@@ -2554,7 +2554,7 @@
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>17</v>
@@ -2585,19 +2585,19 @@
         <v>0.74750000000000005</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L17" s="29">
         <v>203286992</v>
       </c>
       <c r="M17" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="N17" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="N17" s="19" t="s">
+      <c r="O17" s="44" t="s">
         <v>136</v>
-      </c>
-      <c r="O17" s="44" t="s">
-        <v>137</v>
       </c>
       <c r="P17" s="58">
         <f t="shared" si="3"/>
@@ -2614,10 +2614,10 @@
       <c r="S17" s="2">
         <v>2</v>
       </c>
-      <c r="T17" s="82">
+      <c r="T17" s="68">
         <v>5.98</v>
       </c>
-      <c r="U17" s="84">
+      <c r="U17" s="70">
         <f t="shared" si="7"/>
         <v>11.96</v>
       </c>
@@ -2663,8 +2663,8 @@
         <f>$T$1*D18</f>
         <v>0</v>
       </c>
-      <c r="T18" s="82"/>
-      <c r="U18" s="84">
+      <c r="T18" s="68"/>
+      <c r="U18" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2710,8 +2710,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T19" s="82"/>
-      <c r="U19" s="84">
+      <c r="T19" s="68"/>
+      <c r="U19" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2757,8 +2757,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T20" s="82"/>
-      <c r="U20" s="84">
+      <c r="T20" s="68"/>
+      <c r="U20" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2804,8 +2804,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T21" s="82"/>
-      <c r="U21" s="84">
+      <c r="T21" s="68"/>
+      <c r="U21" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2851,8 +2851,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T22" s="82"/>
-      <c r="U22" s="84">
+      <c r="T22" s="68"/>
+      <c r="U22" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2898,8 +2898,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T23" s="82"/>
-      <c r="U23" s="84">
+      <c r="T23" s="68"/>
+      <c r="U23" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2945,8 +2945,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T24" s="82"/>
-      <c r="U24" s="84">
+      <c r="T24" s="68"/>
+      <c r="U24" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -2992,8 +2992,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T25" s="82"/>
-      <c r="U25" s="84">
+      <c r="T25" s="68"/>
+      <c r="U25" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3039,8 +3039,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T26" s="82"/>
-      <c r="U26" s="84">
+      <c r="T26" s="68"/>
+      <c r="U26" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3086,8 +3086,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T27" s="82"/>
-      <c r="U27" s="84">
+      <c r="T27" s="68"/>
+      <c r="U27" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3133,8 +3133,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T28" s="82"/>
-      <c r="U28" s="84">
+      <c r="T28" s="68"/>
+      <c r="U28" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3180,8 +3180,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T29" s="82"/>
-      <c r="U29" s="84">
+      <c r="T29" s="68"/>
+      <c r="U29" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3227,8 +3227,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T30" s="83"/>
-      <c r="U30" s="85">
+      <c r="T30" s="69"/>
+      <c r="U30" s="71">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3269,11 +3269,11 @@
         <v>1</v>
       </c>
       <c r="T31" t="s">
-        <v>157</v>
-      </c>
-      <c r="U31" s="86">
+        <v>156</v>
+      </c>
+      <c r="U31" s="72">
         <f>SUM(U4:U30)</f>
-        <v>3266.8959999999997</v>
+        <v>3571.096</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
@@ -3299,7 +3299,7 @@
         <v>78.965699999999998</v>
       </c>
       <c r="M32" s="30"/>
-      <c r="U32" s="86"/>
+      <c r="U32" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3321,8 +3321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3347,10 +3347,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="71"/>
+      <c r="B1" s="81"/>
       <c r="C1" s="1">
         <v>1</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>44</v>
       </c>
       <c r="S1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T1">
         <f>'Full Instrument'!T1</f>
@@ -3366,50 +3366,50 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="74"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="84"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="72" t="s">
+      <c r="E2" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="75"/>
-      <c r="G2" s="76" t="s">
+      <c r="F2" s="85"/>
+      <c r="G2" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="75"/>
-      <c r="I2" s="72" t="s">
+      <c r="H2" s="85"/>
+      <c r="I2" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="75"/>
-      <c r="K2" s="72" t="s">
+      <c r="J2" s="85"/>
+      <c r="K2" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="73"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="77" t="s">
+      <c r="L2" s="83"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="65" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="65" t="s">
-        <v>150</v>
-      </c>
-      <c r="T2" s="66"/>
-      <c r="U2" s="67"/>
+      <c r="P2" s="75" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="T2" s="76"/>
+      <c r="U2" s="77"/>
     </row>
     <row r="3" spans="1:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>1</v>
@@ -3447,24 +3447,24 @@
       <c r="N3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="78"/>
+      <c r="O3" s="88"/>
       <c r="P3" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q3" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="Q3" s="56" t="s">
+      <c r="R3" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="R3" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="S3" s="80" t="s">
+      <c r="S3" s="66" t="s">
+        <v>150</v>
+      </c>
+      <c r="T3" s="67" t="s">
         <v>151</v>
       </c>
-      <c r="T3" s="81" t="s">
+      <c r="U3" s="65" t="s">
         <v>152</v>
-      </c>
-      <c r="U3" s="79" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -3529,11 +3529,11 @@
       <c r="S4" s="8">
         <v>12</v>
       </c>
-      <c r="T4" s="87">
+      <c r="T4" s="73">
         <f>G4</f>
         <v>9.4499999999999993</v>
       </c>
-      <c r="U4" s="88">
+      <c r="U4" s="74">
         <f>S4*T4</f>
         <v>113.39999999999999</v>
       </c>
@@ -3541,7 +3541,7 @@
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>19</v>
@@ -3599,11 +3599,11 @@
         <f t="shared" ref="S5:S30" si="6">$T$1*D5</f>
         <v>58</v>
       </c>
-      <c r="T5" s="82">
+      <c r="T5" s="68">
         <f>I5</f>
         <v>1.43</v>
       </c>
-      <c r="U5" s="84">
+      <c r="U5" s="70">
         <f t="shared" ref="U5:U30" si="7">S5*T5</f>
         <v>82.94</v>
       </c>
@@ -3611,7 +3611,7 @@
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>22</v>
@@ -3653,7 +3653,7 @@
         <v>25</v>
       </c>
       <c r="O6" s="44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P6" s="58">
         <f t="shared" si="3"/>
@@ -3671,11 +3671,11 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T6" s="82">
+      <c r="T6" s="68">
         <f>E6</f>
         <v>1.39</v>
       </c>
-      <c r="U6" s="84">
+      <c r="U6" s="70">
         <f t="shared" si="7"/>
         <v>80.61999999999999</v>
       </c>
@@ -3683,7 +3683,7 @@
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>38</v>
@@ -3741,11 +3741,11 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T7" s="82">
+      <c r="T7" s="68">
         <f>I7</f>
         <v>0.48</v>
       </c>
-      <c r="U7" s="84">
+      <c r="U7" s="70">
         <f t="shared" si="7"/>
         <v>27.84</v>
       </c>
@@ -3753,7 +3753,7 @@
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>42</v>
@@ -3813,10 +3813,10 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T8" s="82">
+      <c r="T8" s="68">
         <v>0.32700000000000001</v>
       </c>
-      <c r="U8" s="84">
+      <c r="U8" s="70">
         <f t="shared" si="7"/>
         <v>18.966000000000001</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>52</v>
       </c>
       <c r="M9" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N9" s="19" t="s">
         <v>53</v>
@@ -3884,11 +3884,11 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T9" s="82">
+      <c r="T9" s="68">
         <f>I9</f>
         <v>1.43</v>
       </c>
-      <c r="U9" s="84">
+      <c r="U9" s="70">
         <f t="shared" si="7"/>
         <v>82.94</v>
       </c>
@@ -3896,7 +3896,7 @@
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>55</v>
@@ -3956,10 +3956,10 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T10" s="82">
+      <c r="T10" s="68">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="U10" s="84">
+      <c r="U10" s="70">
         <f>S10*T10</f>
         <v>4.5819999999999999</v>
       </c>
@@ -3967,7 +3967,7 @@
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>60</v>
@@ -4027,10 +4027,10 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T11" s="82">
+      <c r="T11" s="68">
         <v>0.86</v>
       </c>
-      <c r="U11" s="84">
+      <c r="U11" s="70">
         <f t="shared" ref="U11:U15" si="11">S11*T11</f>
         <v>49.88</v>
       </c>
@@ -4038,7 +4038,7 @@
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>63</v>
@@ -4071,13 +4071,13 @@
         <v>56</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M12" s="29" t="s">
         <v>17</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O12" s="44" t="s">
         <v>69</v>
@@ -4098,10 +4098,10 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T12" s="82">
+      <c r="T12" s="68">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="U12" s="84">
+      <c r="U12" s="70">
         <f t="shared" si="11"/>
         <v>1.6820000000000002</v>
       </c>
@@ -4109,7 +4109,7 @@
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>66</v>
@@ -4142,13 +4142,13 @@
         <v>56</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M13" s="29" t="s">
         <v>17</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O13" s="44" t="s">
         <v>67</v>
@@ -4169,10 +4169,10 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T13" s="82">
+      <c r="T13" s="68">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="U13" s="84">
+      <c r="U13" s="70">
         <f t="shared" si="11"/>
         <v>0.87</v>
       </c>
@@ -4180,7 +4180,7 @@
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>80</v>
@@ -4213,16 +4213,16 @@
         <v>56</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M14" s="29" t="s">
         <v>17</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O14" s="44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P14" s="58">
         <f t="shared" si="3"/>
@@ -4240,10 +4240,10 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T14" s="82">
+      <c r="T14" s="68">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="U14" s="84">
+      <c r="U14" s="70">
         <f t="shared" si="11"/>
         <v>5.3360000000000003</v>
       </c>
@@ -4251,7 +4251,7 @@
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>81</v>
@@ -4284,16 +4284,16 @@
         <v>56</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M15" s="29" t="s">
         <v>17</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O15" s="44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P15" s="58">
         <f t="shared" si="3"/>
@@ -4311,10 +4311,10 @@
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
-      <c r="T15" s="82">
+      <c r="T15" s="68">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="U15" s="84">
+      <c r="U15" s="70">
         <f t="shared" si="11"/>
         <v>5.3360000000000003</v>
       </c>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="N16" s="27"/>
       <c r="O16" s="44" t="s">
-        <v>84</v>
+        <v>160</v>
       </c>
       <c r="P16" s="58">
         <f t="shared" si="3"/>
@@ -4377,13 +4377,14 @@
         <v>0.36910846110164669</v>
       </c>
       <c r="S16" s="2">
-        <f t="shared" si="6"/>
-        <v>58</v>
-      </c>
-      <c r="T16" s="82"/>
-      <c r="U16" s="84">
+        <v>60</v>
+      </c>
+      <c r="T16" s="68">
+        <v>5.07</v>
+      </c>
+      <c r="U16" s="70">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>304.20000000000005</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
@@ -4427,8 +4428,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T17" s="82"/>
-      <c r="U17" s="84">
+      <c r="T17" s="68"/>
+      <c r="U17" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4474,8 +4475,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T18" s="82"/>
-      <c r="U18" s="84">
+      <c r="T18" s="68"/>
+      <c r="U18" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4521,8 +4522,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T19" s="82"/>
-      <c r="U19" s="84">
+      <c r="T19" s="68"/>
+      <c r="U19" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4568,8 +4569,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T20" s="82"/>
-      <c r="U20" s="84">
+      <c r="T20" s="68"/>
+      <c r="U20" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4615,8 +4616,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T21" s="82"/>
-      <c r="U21" s="84">
+      <c r="T21" s="68"/>
+      <c r="U21" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4662,8 +4663,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T22" s="82"/>
-      <c r="U22" s="84">
+      <c r="T22" s="68"/>
+      <c r="U22" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4709,8 +4710,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T23" s="82"/>
-      <c r="U23" s="84">
+      <c r="T23" s="68"/>
+      <c r="U23" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4756,8 +4757,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T24" s="82"/>
-      <c r="U24" s="84">
+      <c r="T24" s="68"/>
+      <c r="U24" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4803,8 +4804,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T25" s="82"/>
-      <c r="U25" s="84">
+      <c r="T25" s="68"/>
+      <c r="U25" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4850,8 +4851,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T26" s="82"/>
-      <c r="U26" s="84">
+      <c r="T26" s="68"/>
+      <c r="U26" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4897,8 +4898,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T27" s="82"/>
-      <c r="U27" s="84">
+      <c r="T27" s="68"/>
+      <c r="U27" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4944,8 +4945,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T28" s="82"/>
-      <c r="U28" s="84">
+      <c r="T28" s="68"/>
+      <c r="U28" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4991,8 +4992,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T29" s="82"/>
-      <c r="U29" s="84">
+      <c r="T29" s="68"/>
+      <c r="U29" s="70">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5038,8 +5039,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T30" s="83"/>
-      <c r="U30" s="85">
+      <c r="T30" s="69"/>
+      <c r="U30" s="71">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -5079,11 +5080,11 @@
         <v>1</v>
       </c>
       <c r="T31" t="s">
-        <v>157</v>
-      </c>
-      <c r="U31" s="86">
+        <v>156</v>
+      </c>
+      <c r="U31" s="72">
         <f>SUM(U4:U30)</f>
-        <v>474.392</v>
+        <v>778.5920000000001</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
@@ -5108,7 +5109,7 @@
         <f>J31/25</f>
         <v>22.893000000000001</v>
       </c>
-      <c r="U32" s="86"/>
+      <c r="U32" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Moved SHT2x library to main code folder
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1486,7 +1486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>

</xml_diff>